<commit_message>
loadnextleft and right map added display adjusted
</commit_message>
<xml_diff>
--- a/GUI_20212202_AYZ8R9/Maps/map.xlsx
+++ b/GUI_20212202_AYZ8R9/Maps/map.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\game\GUI_20212202_AYZ8R9\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAEE6F99-BA4E-4D7D-927D-2259A76F6C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF8DB7A-C0C3-4603-8A30-50EB062893BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4950" yWindow="1035" windowWidth="21600" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Munka2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="8">
   <si>
     <t>B</t>
   </si>
@@ -112,7 +113,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -148,11 +149,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -168,6 +193,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -450,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AH11" sqref="AH11"/>
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AO34" sqref="AO34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,13 +554,13 @@
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
       <c r="BA1" s="1"/>
-      <c r="BB1" s="1"/>
-      <c r="BC1" s="1"/>
-      <c r="BD1" s="1"/>
-      <c r="BE1" s="1"/>
-      <c r="BF1" s="1"/>
-      <c r="BG1" s="1"/>
-      <c r="BH1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
       <c r="BI1" s="3"/>
       <c r="BJ1" s="3"/>
       <c r="BK1" s="3"/>
@@ -583,13 +620,13 @@
       <c r="AY2" s="1"/>
       <c r="AZ2" s="1"/>
       <c r="BA2" s="1"/>
-      <c r="BB2" s="1"/>
-      <c r="BC2" s="1"/>
-      <c r="BD2" s="1"/>
-      <c r="BE2" s="1"/>
-      <c r="BF2" s="1"/>
-      <c r="BG2" s="1"/>
-      <c r="BH2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
       <c r="BI2" s="3"/>
       <c r="BJ2" s="3"/>
       <c r="BK2" s="3"/>
@@ -649,13 +686,13 @@
       <c r="AY3" s="1"/>
       <c r="AZ3" s="1"/>
       <c r="BA3" s="1"/>
-      <c r="BB3" s="1"/>
-      <c r="BC3" s="1"/>
-      <c r="BD3" s="1"/>
-      <c r="BE3" s="1"/>
-      <c r="BF3" s="1"/>
-      <c r="BG3" s="1"/>
-      <c r="BH3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3"/>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
       <c r="BI3" s="3"/>
       <c r="BJ3" s="3"/>
       <c r="BK3" s="3"/>
@@ -715,13 +752,13 @@
       <c r="AY4" s="1"/>
       <c r="AZ4" s="1"/>
       <c r="BA4" s="1"/>
-      <c r="BB4" s="1"/>
-      <c r="BC4" s="1"/>
-      <c r="BD4" s="1"/>
-      <c r="BE4" s="1"/>
-      <c r="BF4" s="1"/>
-      <c r="BG4" s="1"/>
-      <c r="BH4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="3"/>
+      <c r="BD4" s="3"/>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3"/>
+      <c r="BG4" s="3"/>
+      <c r="BH4" s="3"/>
       <c r="BI4" s="3"/>
       <c r="BJ4" s="3"/>
       <c r="BK4" s="3"/>
@@ -781,13 +818,13 @@
       <c r="AY5" s="1"/>
       <c r="AZ5" s="1"/>
       <c r="BA5" s="1"/>
-      <c r="BB5" s="1"/>
-      <c r="BC5" s="1"/>
-      <c r="BD5" s="1"/>
-      <c r="BE5" s="1"/>
-      <c r="BF5" s="1"/>
-      <c r="BG5" s="1"/>
-      <c r="BH5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="3"/>
+      <c r="BD5" s="3"/>
+      <c r="BE5" s="3"/>
+      <c r="BF5" s="3"/>
+      <c r="BG5" s="3"/>
+      <c r="BH5" s="3"/>
       <c r="BI5" s="3"/>
       <c r="BJ5" s="3"/>
       <c r="BK5" s="3"/>
@@ -847,13 +884,13 @@
       <c r="AY6" s="1"/>
       <c r="AZ6" s="1"/>
       <c r="BA6" s="1"/>
-      <c r="BB6" s="1"/>
-      <c r="BC6" s="1"/>
-      <c r="BD6" s="1"/>
-      <c r="BE6" s="1"/>
-      <c r="BF6" s="1"/>
-      <c r="BG6" s="1"/>
-      <c r="BH6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="3"/>
+      <c r="BD6" s="3"/>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3"/>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="3"/>
       <c r="BI6" s="3"/>
       <c r="BJ6" s="3"/>
       <c r="BK6" s="3"/>
@@ -913,13 +950,13 @@
       <c r="AY7" s="1"/>
       <c r="AZ7" s="1"/>
       <c r="BA7" s="1"/>
-      <c r="BB7" s="1"/>
-      <c r="BC7" s="1"/>
-      <c r="BD7" s="1"/>
-      <c r="BE7" s="1"/>
-      <c r="BF7" s="1"/>
-      <c r="BG7" s="1"/>
-      <c r="BH7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="3"/>
+      <c r="BD7" s="3"/>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
       <c r="BI7" s="3"/>
       <c r="BJ7" s="3"/>
       <c r="BK7" s="3"/>
@@ -979,13 +1016,13 @@
       <c r="AY8" s="1"/>
       <c r="AZ8" s="1"/>
       <c r="BA8" s="1"/>
-      <c r="BB8" s="1"/>
-      <c r="BC8" s="1"/>
-      <c r="BD8" s="1"/>
-      <c r="BE8" s="1"/>
-      <c r="BF8" s="1"/>
-      <c r="BG8" s="1"/>
-      <c r="BH8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="3"/>
+      <c r="BD8" s="3"/>
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3"/>
+      <c r="BG8" s="3"/>
+      <c r="BH8" s="3"/>
       <c r="BI8" s="3"/>
       <c r="BJ8" s="3"/>
       <c r="BK8" s="3"/>
@@ -1045,13 +1082,13 @@
       <c r="AY9" s="1"/>
       <c r="AZ9" s="1"/>
       <c r="BA9" s="1"/>
-      <c r="BB9" s="1"/>
-      <c r="BC9" s="1"/>
-      <c r="BD9" s="1"/>
-      <c r="BE9" s="1"/>
-      <c r="BF9" s="1"/>
-      <c r="BG9" s="1"/>
-      <c r="BH9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="3"/>
+      <c r="BD9" s="3"/>
+      <c r="BE9" s="3"/>
+      <c r="BF9" s="3"/>
+      <c r="BG9" s="3"/>
+      <c r="BH9" s="3"/>
       <c r="BI9" s="3"/>
       <c r="BJ9" s="3"/>
       <c r="BK9" s="3"/>
@@ -1111,13 +1148,13 @@
       <c r="AY10" s="1"/>
       <c r="AZ10" s="1"/>
       <c r="BA10" s="1"/>
-      <c r="BB10" s="1"/>
-      <c r="BC10" s="1"/>
-      <c r="BD10" s="1"/>
-      <c r="BE10" s="1"/>
-      <c r="BF10" s="1"/>
-      <c r="BG10" s="1"/>
-      <c r="BH10" s="2"/>
+      <c r="BB10" s="2"/>
+      <c r="BC10" s="3"/>
+      <c r="BD10" s="3"/>
+      <c r="BE10" s="3"/>
+      <c r="BF10" s="3"/>
+      <c r="BG10" s="3"/>
+      <c r="BH10" s="3"/>
       <c r="BI10" s="3"/>
       <c r="BJ10" s="3"/>
       <c r="BK10" s="3"/>
@@ -1177,13 +1214,13 @@
       <c r="AY11" s="1"/>
       <c r="AZ11" s="1"/>
       <c r="BA11" s="1"/>
-      <c r="BB11" s="1"/>
-      <c r="BC11" s="1"/>
-      <c r="BD11" s="1"/>
-      <c r="BE11" s="1"/>
-      <c r="BF11" s="1"/>
-      <c r="BG11" s="1"/>
-      <c r="BH11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="3"/>
+      <c r="BD11" s="3"/>
+      <c r="BE11" s="3"/>
+      <c r="BF11" s="3"/>
+      <c r="BG11" s="3"/>
+      <c r="BH11" s="3"/>
       <c r="BI11" s="3"/>
       <c r="BJ11" s="3"/>
       <c r="BK11" s="3"/>
@@ -1243,13 +1280,13 @@
       <c r="AY12" s="1"/>
       <c r="AZ12" s="1"/>
       <c r="BA12" s="1"/>
-      <c r="BB12" s="1"/>
-      <c r="BC12" s="1"/>
-      <c r="BD12" s="1"/>
-      <c r="BE12" s="1"/>
-      <c r="BF12" s="1"/>
-      <c r="BG12" s="1"/>
-      <c r="BH12" s="2"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="3"/>
+      <c r="BD12" s="3"/>
+      <c r="BE12" s="3"/>
+      <c r="BF12" s="3"/>
+      <c r="BG12" s="3"/>
+      <c r="BH12" s="3"/>
       <c r="BI12" s="3"/>
       <c r="BJ12" s="3"/>
       <c r="BK12" s="3"/>
@@ -1331,13 +1368,13 @@
       <c r="AY13" s="1"/>
       <c r="AZ13" s="1"/>
       <c r="BA13" s="1"/>
-      <c r="BB13" s="1"/>
-      <c r="BC13" s="1"/>
-      <c r="BD13" s="1"/>
-      <c r="BE13" s="1"/>
-      <c r="BF13" s="1"/>
-      <c r="BG13" s="1"/>
-      <c r="BH13" s="2"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3"/>
+      <c r="BG13" s="3"/>
+      <c r="BH13" s="3"/>
       <c r="BI13" s="3"/>
       <c r="BJ13" s="3"/>
       <c r="BK13" s="3"/>
@@ -1403,13 +1440,13 @@
       <c r="AY14" s="1"/>
       <c r="AZ14" s="1"/>
       <c r="BA14" s="1"/>
-      <c r="BB14" s="1"/>
-      <c r="BC14" s="1"/>
-      <c r="BD14" s="1"/>
-      <c r="BE14" s="1"/>
-      <c r="BF14" s="1"/>
-      <c r="BG14" s="1"/>
-      <c r="BH14" s="2"/>
+      <c r="BB14" s="2"/>
+      <c r="BC14" s="3"/>
+      <c r="BD14" s="3"/>
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
       <c r="BI14" s="3"/>
       <c r="BJ14" s="3"/>
       <c r="BK14" s="3"/>
@@ -1475,13 +1512,13 @@
       <c r="AY15" s="1"/>
       <c r="AZ15" s="1"/>
       <c r="BA15" s="1"/>
-      <c r="BB15" s="1"/>
-      <c r="BC15" s="1"/>
-      <c r="BD15" s="1"/>
-      <c r="BE15" s="1"/>
-      <c r="BF15" s="1"/>
-      <c r="BG15" s="1"/>
-      <c r="BH15" s="2"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="3"/>
+      <c r="BD15" s="3"/>
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3"/>
+      <c r="BG15" s="3"/>
+      <c r="BH15" s="3"/>
       <c r="BI15" s="3"/>
       <c r="BJ15" s="3"/>
       <c r="BK15" s="3"/>
@@ -1561,13 +1598,13 @@
       <c r="AY16" s="1"/>
       <c r="AZ16" s="1"/>
       <c r="BA16" s="1"/>
-      <c r="BB16" s="1"/>
-      <c r="BC16" s="1"/>
-      <c r="BD16" s="1"/>
-      <c r="BE16" s="1"/>
-      <c r="BF16" s="1"/>
-      <c r="BG16" s="1"/>
-      <c r="BH16" s="2"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="3"/>
+      <c r="BD16" s="3"/>
+      <c r="BE16" s="3"/>
+      <c r="BF16" s="3"/>
+      <c r="BG16" s="3"/>
+      <c r="BH16" s="3"/>
       <c r="BI16" s="3"/>
       <c r="BJ16" s="3"/>
       <c r="BK16" s="3"/>
@@ -1635,13 +1672,13 @@
       <c r="AY17" s="1"/>
       <c r="AZ17" s="1"/>
       <c r="BA17" s="1"/>
-      <c r="BB17" s="1"/>
-      <c r="BC17" s="1"/>
-      <c r="BD17" s="1"/>
-      <c r="BE17" s="1"/>
-      <c r="BF17" s="1"/>
-      <c r="BG17" s="1"/>
-      <c r="BH17" s="2"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="3"/>
+      <c r="BD17" s="3"/>
+      <c r="BE17" s="3"/>
+      <c r="BF17" s="3"/>
+      <c r="BG17" s="3"/>
+      <c r="BH17" s="3"/>
       <c r="BI17" s="3"/>
       <c r="BJ17" s="3"/>
       <c r="BK17" s="3"/>
@@ -1727,13 +1764,13 @@
       <c r="AY18" s="1"/>
       <c r="AZ18" s="1"/>
       <c r="BA18" s="1"/>
-      <c r="BB18" s="1"/>
-      <c r="BC18" s="1"/>
-      <c r="BD18" s="1"/>
-      <c r="BE18" s="1"/>
-      <c r="BF18" s="1"/>
-      <c r="BG18" s="1"/>
-      <c r="BH18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="3"/>
+      <c r="BD18" s="3"/>
+      <c r="BE18" s="3"/>
+      <c r="BF18" s="3"/>
+      <c r="BG18" s="3"/>
+      <c r="BH18" s="3"/>
       <c r="BI18" s="3"/>
       <c r="BJ18" s="3"/>
       <c r="BK18" s="3"/>
@@ -1796,7 +1833,12 @@
       <c r="AT19" t="s">
         <v>2</v>
       </c>
-      <c r="BH19" s="2"/>
+      <c r="BC19" s="3"/>
+      <c r="BD19" s="3"/>
+      <c r="BE19" s="3"/>
+      <c r="BF19" s="3"/>
+      <c r="BG19" s="3"/>
+      <c r="BH19" s="3"/>
       <c r="BI19" s="3"/>
       <c r="BJ19" s="3"/>
       <c r="BK19" s="3"/>
@@ -1878,15 +1920,15 @@
       <c r="BA20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BB20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BC20" s="1"/>
-      <c r="BD20" s="1"/>
-      <c r="BE20" s="1"/>
-      <c r="BF20" s="1"/>
-      <c r="BG20" s="1"/>
-      <c r="BH20" s="1"/>
+      <c r="BB20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="3"/>
+      <c r="BD20" s="3"/>
+      <c r="BE20" s="3"/>
+      <c r="BF20" s="3"/>
+      <c r="BG20" s="3"/>
+      <c r="BH20" s="3"/>
       <c r="BI20" s="3"/>
       <c r="BJ20" s="3"/>
       <c r="BK20" s="3"/>
@@ -1952,16 +1994,13 @@
       <c r="AY21" s="1"/>
       <c r="AZ21" s="1"/>
       <c r="BA21" s="1"/>
-      <c r="BB21" s="1"/>
-      <c r="BC21" s="1"/>
-      <c r="BD21" s="1" t="str">
-        <f>IF(BB20="Z","Z",IF(AND(BB20&lt;&gt;"U",BB20&lt;&gt;"V",BB20&lt;&gt;"W"),"V",IF(BB20="V","U",IF(BB20="U","W",IF(BB20="W","Z",IF(BB20="Z","",""))))))</f>
-        <v>V</v>
-      </c>
-      <c r="BE21" s="1"/>
-      <c r="BF21" s="1"/>
-      <c r="BG21" s="1"/>
-      <c r="BH21" s="1"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="3"/>
+      <c r="BD21" s="3"/>
+      <c r="BE21" s="3"/>
+      <c r="BF21" s="3"/>
+      <c r="BG21" s="3"/>
+      <c r="BH21" s="3"/>
       <c r="BI21" s="3"/>
       <c r="BJ21" s="3"/>
       <c r="BK21" s="3"/>
@@ -2027,13 +2066,13 @@
       <c r="AY22" s="1"/>
       <c r="AZ22" s="1"/>
       <c r="BA22" s="1"/>
-      <c r="BB22" s="1"/>
-      <c r="BC22" s="1"/>
-      <c r="BD22" s="1"/>
-      <c r="BE22" s="1"/>
-      <c r="BF22" s="1"/>
-      <c r="BG22" s="1"/>
-      <c r="BH22" s="1"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="3"/>
+      <c r="BD22" s="3"/>
+      <c r="BE22" s="3"/>
+      <c r="BF22" s="3"/>
+      <c r="BG22" s="3"/>
+      <c r="BH22" s="3"/>
       <c r="BI22" s="3"/>
       <c r="BJ22" s="3"/>
       <c r="BK22" s="3"/>
@@ -2099,13 +2138,13 @@
       <c r="AY23" s="1"/>
       <c r="AZ23" s="1"/>
       <c r="BA23" s="1"/>
-      <c r="BB23" s="1"/>
-      <c r="BC23" s="1"/>
-      <c r="BD23" s="1"/>
-      <c r="BE23" s="1"/>
-      <c r="BF23" s="1"/>
-      <c r="BG23" s="1"/>
-      <c r="BH23" s="1"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="3"/>
+      <c r="BD23" s="3"/>
+      <c r="BE23" s="3"/>
+      <c r="BF23" s="3"/>
+      <c r="BG23" s="3"/>
+      <c r="BH23" s="3"/>
       <c r="BI23" s="3"/>
       <c r="BJ23" s="3"/>
       <c r="BK23" s="3"/>
@@ -2183,13 +2222,13 @@
       <c r="AY24" s="1"/>
       <c r="AZ24" s="1"/>
       <c r="BA24" s="1"/>
-      <c r="BB24" s="1"/>
-      <c r="BC24" s="1"/>
-      <c r="BD24" s="1"/>
-      <c r="BE24" s="1"/>
-      <c r="BF24" s="1"/>
-      <c r="BG24" s="1"/>
-      <c r="BH24" s="1"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="3"/>
+      <c r="BD24" s="3"/>
+      <c r="BE24" s="3"/>
+      <c r="BF24" s="3"/>
+      <c r="BG24" s="3"/>
+      <c r="BH24" s="3"/>
       <c r="BI24" s="3"/>
       <c r="BJ24" s="3"/>
       <c r="BK24" s="3"/>
@@ -2249,13 +2288,13 @@
       <c r="AY25" s="1"/>
       <c r="AZ25" s="1"/>
       <c r="BA25" s="1"/>
-      <c r="BB25" s="1"/>
-      <c r="BC25" s="1"/>
-      <c r="BD25" s="1"/>
-      <c r="BE25" s="1"/>
-      <c r="BF25" s="1"/>
-      <c r="BG25" s="1"/>
-      <c r="BH25" s="1"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="3"/>
+      <c r="BD25" s="3"/>
+      <c r="BE25" s="3"/>
+      <c r="BF25" s="3"/>
+      <c r="BG25" s="3"/>
+      <c r="BH25" s="3"/>
       <c r="BI25" s="3"/>
       <c r="BJ25" s="3"/>
       <c r="BK25" s="3"/>
@@ -2315,13 +2354,13 @@
       <c r="AY26" s="1"/>
       <c r="AZ26" s="1"/>
       <c r="BA26" s="1"/>
-      <c r="BB26" s="1"/>
-      <c r="BC26" s="1"/>
-      <c r="BD26" s="1"/>
-      <c r="BE26" s="1"/>
-      <c r="BF26" s="1"/>
-      <c r="BG26" s="1"/>
-      <c r="BH26" s="1"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="3"/>
+      <c r="BD26" s="3"/>
+      <c r="BE26" s="3"/>
+      <c r="BF26" s="3"/>
+      <c r="BG26" s="3"/>
+      <c r="BH26" s="3"/>
       <c r="BI26" s="3"/>
       <c r="BJ26" s="3"/>
       <c r="BK26" s="3"/>
@@ -2380,13 +2419,13 @@
       <c r="AY27" s="1"/>
       <c r="AZ27" s="1"/>
       <c r="BA27" s="1"/>
-      <c r="BB27" s="1"/>
-      <c r="BC27" s="1"/>
-      <c r="BD27" s="1"/>
-      <c r="BE27" s="1"/>
-      <c r="BF27" s="1"/>
-      <c r="BG27" s="1"/>
-      <c r="BH27" s="1"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="3"/>
+      <c r="BD27" s="3"/>
+      <c r="BE27" s="3"/>
+      <c r="BF27" s="3"/>
+      <c r="BG27" s="3"/>
+      <c r="BH27" s="3"/>
       <c r="BI27" s="3"/>
       <c r="BJ27" s="3"/>
       <c r="BK27" s="3"/>
@@ -2446,13 +2485,13 @@
       <c r="AY28" s="1"/>
       <c r="AZ28" s="1"/>
       <c r="BA28" s="1"/>
-      <c r="BB28" s="1"/>
-      <c r="BC28" s="1"/>
-      <c r="BD28" s="1"/>
-      <c r="BE28" s="1"/>
-      <c r="BF28" s="1"/>
-      <c r="BG28" s="1"/>
-      <c r="BH28" s="1"/>
+      <c r="BB28" s="2"/>
+      <c r="BC28" s="3"/>
+      <c r="BD28" s="3"/>
+      <c r="BE28" s="3"/>
+      <c r="BF28" s="3"/>
+      <c r="BG28" s="3"/>
+      <c r="BH28" s="3"/>
       <c r="BI28" s="3"/>
       <c r="BJ28" s="3"/>
       <c r="BK28" s="3"/>
@@ -2512,343 +2551,343 @@
       <c r="AY29" s="1"/>
       <c r="AZ29" s="1"/>
       <c r="BA29" s="1"/>
-      <c r="BB29" s="1"/>
-      <c r="BC29" s="1"/>
-      <c r="BD29" s="1"/>
-      <c r="BE29" s="1"/>
-      <c r="BF29" s="1"/>
-      <c r="BG29" s="1"/>
-      <c r="BH29" s="1"/>
+      <c r="BB29" s="2"/>
+      <c r="BC29" s="3"/>
+      <c r="BD29" s="3"/>
+      <c r="BE29" s="3"/>
+      <c r="BF29" s="3"/>
+      <c r="BG29" s="3"/>
+      <c r="BH29" s="3"/>
       <c r="BI29" s="3"/>
       <c r="BJ29" s="3"/>
       <c r="BK29" s="3"/>
       <c r="BL29" s="3"/>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
-      <c r="N30" s="1"/>
-      <c r="O30" s="1"/>
-      <c r="P30" s="1"/>
-      <c r="Q30" s="1"/>
-      <c r="R30" s="1"/>
-      <c r="S30" s="1"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="1"/>
-      <c r="V30" s="1"/>
-      <c r="W30" s="1"/>
-      <c r="X30" s="1"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
-      <c r="AD30" s="9"/>
-      <c r="AE30" s="1"/>
-      <c r="AF30" s="1"/>
-      <c r="AG30" s="1"/>
-      <c r="AH30" s="1"/>
-      <c r="AI30" s="1"/>
-      <c r="AJ30" s="1"/>
-      <c r="AK30" s="1"/>
-      <c r="AL30" s="1"/>
-      <c r="AM30" s="1"/>
-      <c r="AN30" s="11"/>
-      <c r="AO30" s="1"/>
-      <c r="AP30" s="1"/>
-      <c r="AQ30" s="1"/>
-      <c r="AR30" s="1"/>
-      <c r="AS30" s="1"/>
-      <c r="AT30" s="1"/>
-      <c r="AU30" s="1"/>
-      <c r="AV30" s="1"/>
-      <c r="AW30" s="1"/>
-      <c r="AX30" s="13"/>
-      <c r="AY30" s="1"/>
-      <c r="AZ30" s="1"/>
-      <c r="BA30" s="1"/>
-      <c r="BB30" s="1"/>
-      <c r="BC30" s="1"/>
-      <c r="BD30" s="1"/>
-      <c r="BE30" s="1"/>
-      <c r="BF30" s="1"/>
-      <c r="BG30" s="1"/>
-      <c r="BH30" s="1"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="15"/>
+      <c r="AC30" s="15"/>
+      <c r="AD30" s="18"/>
+      <c r="AE30" s="15"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="15"/>
+      <c r="AH30" s="15"/>
+      <c r="AI30" s="15"/>
+      <c r="AJ30" s="15"/>
+      <c r="AK30" s="15"/>
+      <c r="AL30" s="15"/>
+      <c r="AM30" s="15"/>
+      <c r="AN30" s="22"/>
+      <c r="AO30" s="15"/>
+      <c r="AP30" s="15"/>
+      <c r="AQ30" s="15"/>
+      <c r="AR30" s="15"/>
+      <c r="AS30" s="15"/>
+      <c r="AT30" s="15"/>
+      <c r="AU30" s="15"/>
+      <c r="AV30" s="15"/>
+      <c r="AW30" s="15"/>
+      <c r="AX30" s="23"/>
+      <c r="AY30" s="15"/>
+      <c r="AZ30" s="15"/>
+      <c r="BA30" s="15"/>
+      <c r="BB30" s="24"/>
+      <c r="BC30" s="3"/>
+      <c r="BD30" s="3"/>
+      <c r="BE30" s="3"/>
+      <c r="BF30" s="3"/>
+      <c r="BG30" s="3"/>
+      <c r="BH30" s="3"/>
       <c r="BI30" s="3"/>
       <c r="BJ30" s="3"/>
       <c r="BK30" s="3"/>
       <c r="BL30" s="3"/>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
-      <c r="O31" s="1"/>
-      <c r="P31" s="1"/>
-      <c r="Q31" s="1"/>
-      <c r="R31" s="1"/>
-      <c r="S31" s="1"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="1"/>
-      <c r="V31" s="1"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-      <c r="Y31" s="1"/>
-      <c r="Z31" s="1"/>
-      <c r="AA31" s="1"/>
-      <c r="AB31" s="1"/>
-      <c r="AC31" s="1"/>
-      <c r="AD31" s="9"/>
-      <c r="AE31" s="1"/>
-      <c r="AF31" s="1"/>
-      <c r="AG31" s="1"/>
-      <c r="AH31" s="1"/>
-      <c r="AI31" s="1"/>
-      <c r="AJ31" s="1"/>
-      <c r="AK31" s="1"/>
-      <c r="AL31" s="1"/>
-      <c r="AM31" s="1"/>
-      <c r="AN31" s="11"/>
-      <c r="AO31" s="1"/>
-      <c r="AP31" s="1"/>
-      <c r="AQ31" s="1"/>
-      <c r="AR31" s="1"/>
-      <c r="AS31" s="1"/>
-      <c r="AT31" s="1"/>
-      <c r="AU31" s="1"/>
-      <c r="AV31" s="1"/>
-      <c r="AW31" s="1"/>
-      <c r="AX31" s="13"/>
-      <c r="AY31" s="1"/>
-      <c r="AZ31" s="1"/>
-      <c r="BA31" s="1"/>
-      <c r="BB31" s="1"/>
-      <c r="BC31" s="1"/>
-      <c r="BD31" s="1"/>
-      <c r="BE31" s="1"/>
-      <c r="BF31" s="1"/>
-      <c r="BG31" s="1"/>
-      <c r="BH31" s="1"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="21"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
+      <c r="AN31" s="25"/>
+      <c r="AO31" s="3"/>
+      <c r="AP31" s="3"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="3"/>
+      <c r="AU31" s="3"/>
+      <c r="AV31" s="3"/>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="26"/>
+      <c r="AY31" s="3"/>
+      <c r="AZ31" s="3"/>
+      <c r="BA31" s="3"/>
+      <c r="BB31" s="3"/>
+      <c r="BC31" s="3"/>
+      <c r="BD31" s="3"/>
+      <c r="BE31" s="3"/>
+      <c r="BF31" s="3"/>
+      <c r="BG31" s="3"/>
+      <c r="BH31" s="3"/>
       <c r="BI31" s="3"/>
       <c r="BJ31" s="3"/>
       <c r="BK31" s="3"/>
       <c r="BL31" s="3"/>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
-      <c r="P32" s="1"/>
-      <c r="Q32" s="1"/>
-      <c r="R32" s="1"/>
-      <c r="S32" s="1"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="1"/>
-      <c r="V32" s="1"/>
-      <c r="W32" s="1"/>
-      <c r="X32" s="1"/>
-      <c r="Y32" s="1"/>
-      <c r="Z32" s="1"/>
-      <c r="AA32" s="1"/>
-      <c r="AB32" s="1"/>
-      <c r="AC32" s="1"/>
-      <c r="AD32" s="9"/>
-      <c r="AE32" s="1"/>
-      <c r="AF32" s="1"/>
-      <c r="AG32" s="1"/>
-      <c r="AH32" s="1"/>
-      <c r="AI32" s="1"/>
-      <c r="AJ32" s="1"/>
-      <c r="AK32" s="1"/>
-      <c r="AL32" s="1"/>
-      <c r="AM32" s="1"/>
-      <c r="AN32" s="11"/>
-      <c r="AO32" s="1"/>
-      <c r="AP32" s="1"/>
-      <c r="AQ32" s="1"/>
-      <c r="AR32" s="1"/>
-      <c r="AS32" s="1"/>
-      <c r="AT32" s="1"/>
-      <c r="AU32" s="1"/>
-      <c r="AV32" s="1"/>
-      <c r="AW32" s="1"/>
-      <c r="AX32" s="13"/>
-      <c r="AY32" s="1"/>
-      <c r="AZ32" s="1"/>
-      <c r="BA32" s="1"/>
-      <c r="BB32" s="1"/>
-      <c r="BC32" s="1"/>
-      <c r="BD32" s="1"/>
-      <c r="BE32" s="1"/>
-      <c r="BF32" s="1"/>
-      <c r="BG32" s="1"/>
-      <c r="BH32" s="1"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
+      <c r="AM32" s="3"/>
+      <c r="AN32" s="25"/>
+      <c r="AO32" s="3"/>
+      <c r="AP32" s="3"/>
+      <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
+      <c r="AS32" s="3"/>
+      <c r="AT32" s="3"/>
+      <c r="AU32" s="3"/>
+      <c r="AV32" s="3"/>
+      <c r="AW32" s="3"/>
+      <c r="AX32" s="26"/>
+      <c r="AY32" s="3"/>
+      <c r="AZ32" s="3"/>
+      <c r="BA32" s="3"/>
+      <c r="BB32" s="3"/>
+      <c r="BC32" s="3"/>
+      <c r="BD32" s="3"/>
+      <c r="BE32" s="3"/>
+      <c r="BF32" s="3"/>
+      <c r="BG32" s="3"/>
+      <c r="BH32" s="3"/>
       <c r="BI32" s="3"/>
       <c r="BJ32" s="3"/>
       <c r="BK32" s="3"/>
       <c r="BL32" s="3"/>
     </row>
     <row r="33" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="1"/>
-      <c r="S33" s="1"/>
-      <c r="T33" s="7"/>
-      <c r="U33" s="1"/>
-      <c r="V33" s="1"/>
-      <c r="W33" s="1"/>
-      <c r="X33" s="1"/>
-      <c r="Y33" s="1"/>
-      <c r="Z33" s="1"/>
-      <c r="AA33" s="1"/>
-      <c r="AB33" s="1"/>
-      <c r="AC33" s="1"/>
-      <c r="AD33" s="9"/>
-      <c r="AE33" s="1"/>
-      <c r="AF33" s="1"/>
-      <c r="AG33" s="1"/>
-      <c r="AH33" s="1"/>
-      <c r="AI33" s="1"/>
-      <c r="AJ33" s="1"/>
-      <c r="AK33" s="1"/>
-      <c r="AL33" s="1"/>
-      <c r="AM33" s="1"/>
-      <c r="AN33" s="11"/>
-      <c r="AO33" s="1"/>
-      <c r="AP33" s="1"/>
-      <c r="AQ33" s="1"/>
-      <c r="AR33" s="1"/>
-      <c r="AS33" s="1"/>
-      <c r="AT33" s="1"/>
-      <c r="AU33" s="1"/>
-      <c r="AV33" s="1"/>
-      <c r="AW33" s="1"/>
-      <c r="AX33" s="13"/>
-      <c r="AY33" s="1"/>
-      <c r="AZ33" s="1"/>
-      <c r="BA33" s="1"/>
-      <c r="BB33" s="1"/>
-      <c r="BC33" s="1"/>
-      <c r="BD33" s="1"/>
-      <c r="BE33" s="1"/>
-      <c r="BF33" s="1"/>
-      <c r="BG33" s="1"/>
-      <c r="BH33" s="1"/>
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="21"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="3"/>
+      <c r="AM33" s="3"/>
+      <c r="AN33" s="25"/>
+      <c r="AO33" s="3"/>
+      <c r="AP33" s="3"/>
+      <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
+      <c r="AS33" s="3"/>
+      <c r="AT33" s="3"/>
+      <c r="AU33" s="3"/>
+      <c r="AV33" s="3"/>
+      <c r="AW33" s="3"/>
+      <c r="AX33" s="26"/>
+      <c r="AY33" s="3"/>
+      <c r="AZ33" s="3"/>
+      <c r="BA33" s="3"/>
+      <c r="BB33" s="3"/>
+      <c r="BC33" s="3"/>
+      <c r="BD33" s="3"/>
+      <c r="BE33" s="3"/>
+      <c r="BF33" s="3"/>
+      <c r="BG33" s="3"/>
+      <c r="BH33" s="3"/>
       <c r="BI33" s="3"/>
       <c r="BJ33" s="3"/>
       <c r="BK33" s="3"/>
       <c r="BL33" s="3"/>
     </row>
     <row r="34" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="1"/>
-      <c r="S34" s="1"/>
-      <c r="T34" s="7"/>
-      <c r="U34" s="1"/>
-      <c r="V34" s="1"/>
-      <c r="W34" s="1"/>
-      <c r="X34" s="1"/>
-      <c r="Y34" s="1"/>
-      <c r="Z34" s="1"/>
-      <c r="AA34" s="1"/>
-      <c r="AB34" s="1"/>
-      <c r="AC34" s="1"/>
-      <c r="AD34" s="9"/>
-      <c r="AE34" s="1"/>
-      <c r="AF34" s="1"/>
-      <c r="AG34" s="1"/>
-      <c r="AH34" s="1"/>
-      <c r="AI34" s="1"/>
-      <c r="AJ34" s="1"/>
-      <c r="AK34" s="1"/>
-      <c r="AL34" s="1"/>
-      <c r="AM34" s="1"/>
-      <c r="AN34" s="11"/>
-      <c r="AO34" s="1"/>
-      <c r="AP34" s="1"/>
-      <c r="AQ34" s="1"/>
-      <c r="AR34" s="1"/>
-      <c r="AS34" s="1"/>
-      <c r="AT34" s="1"/>
-      <c r="AU34" s="1"/>
-      <c r="AV34" s="1"/>
-      <c r="AW34" s="1"/>
-      <c r="AX34" s="13"/>
-      <c r="AY34" s="1"/>
-      <c r="AZ34" s="1"/>
-      <c r="BA34" s="1"/>
-      <c r="BB34" s="1"/>
-      <c r="BC34" s="1"/>
-      <c r="BD34" s="1"/>
-      <c r="BE34" s="1"/>
-      <c r="BF34" s="1"/>
-      <c r="BG34" s="1"/>
-      <c r="BH34" s="1"/>
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="21"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3"/>
+      <c r="AL34" s="3"/>
+      <c r="AM34" s="3"/>
+      <c r="AN34" s="25"/>
+      <c r="AO34" s="3"/>
+      <c r="AP34" s="3"/>
+      <c r="AQ34" s="3"/>
+      <c r="AR34" s="3"/>
+      <c r="AS34" s="3"/>
+      <c r="AT34" s="3"/>
+      <c r="AU34" s="3"/>
+      <c r="AV34" s="3"/>
+      <c r="AW34" s="3"/>
+      <c r="AX34" s="26"/>
+      <c r="AY34" s="3"/>
+      <c r="AZ34" s="3"/>
+      <c r="BA34" s="3"/>
+      <c r="BB34" s="3"/>
+      <c r="BC34" s="3"/>
+      <c r="BD34" s="3"/>
+      <c r="BE34" s="3"/>
+      <c r="BF34" s="3"/>
+      <c r="BG34" s="3"/>
+      <c r="BH34" s="3"/>
       <c r="BI34" s="3"/>
       <c r="BJ34" s="3"/>
       <c r="BK34" s="3"/>
@@ -2868,4 +2907,2490 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32EA023-0038-482A-B633-0391C0CB8525}">
+  <dimension ref="A1:BL34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AZ28" sqref="AZ28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="9.140625" style="6"/>
+    <col min="20" max="20" width="9.140625" style="8"/>
+    <col min="30" max="30" width="9.140625" style="10"/>
+    <col min="40" max="40" width="9.140625" style="12"/>
+    <col min="50" max="50" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
+      <c r="BI1" s="3"/>
+      <c r="BJ1" s="3"/>
+      <c r="BK1" s="3"/>
+      <c r="BL1" s="3"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="13"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
+      <c r="BI2" s="3"/>
+      <c r="BJ2" s="3"/>
+      <c r="BK2" s="3"/>
+      <c r="BL2" s="3"/>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="13"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3"/>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
+      <c r="BI3" s="3"/>
+      <c r="BJ3" s="3"/>
+      <c r="BK3" s="3"/>
+      <c r="BL3" s="3"/>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="3"/>
+      <c r="BD4" s="3"/>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3"/>
+      <c r="BG4" s="3"/>
+      <c r="BH4" s="3"/>
+      <c r="BI4" s="3"/>
+      <c r="BJ4" s="3"/>
+      <c r="BK4" s="3"/>
+      <c r="BL4" s="3"/>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="11"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="13"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="3"/>
+      <c r="BD5" s="3"/>
+      <c r="BE5" s="3"/>
+      <c r="BF5" s="3"/>
+      <c r="BG5" s="3"/>
+      <c r="BH5" s="3"/>
+      <c r="BI5" s="3"/>
+      <c r="BJ5" s="3"/>
+      <c r="BK5" s="3"/>
+      <c r="BL5" s="3"/>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="13"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="3"/>
+      <c r="BD6" s="3"/>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3"/>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="3"/>
+      <c r="BI6" s="3"/>
+      <c r="BJ6" s="3"/>
+      <c r="BK6" s="3"/>
+      <c r="BL6" s="3"/>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="13"/>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="3"/>
+      <c r="BD7" s="3"/>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
+      <c r="BI7" s="3"/>
+      <c r="BJ7" s="3"/>
+      <c r="BK7" s="3"/>
+      <c r="BL7" s="3"/>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="13"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="3"/>
+      <c r="BD8" s="3"/>
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3"/>
+      <c r="BG8" s="3"/>
+      <c r="BH8" s="3"/>
+      <c r="BI8" s="3"/>
+      <c r="BJ8" s="3"/>
+      <c r="BK8" s="3"/>
+      <c r="BL8" s="3"/>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="13"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="3"/>
+      <c r="BD9" s="3"/>
+      <c r="BE9" s="3"/>
+      <c r="BF9" s="3"/>
+      <c r="BG9" s="3"/>
+      <c r="BH9" s="3"/>
+      <c r="BI9" s="3"/>
+      <c r="BJ9" s="3"/>
+      <c r="BK9" s="3"/>
+      <c r="BL9" s="3"/>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC10" s="3"/>
+      <c r="BD10" s="3"/>
+      <c r="BE10" s="3"/>
+      <c r="BF10" s="3"/>
+      <c r="BG10" s="3"/>
+      <c r="BH10" s="3"/>
+      <c r="BI10" s="3"/>
+      <c r="BJ10" s="3"/>
+      <c r="BK10" s="3"/>
+      <c r="BL10" s="3"/>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX11" s="13"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="3"/>
+      <c r="BD11" s="3"/>
+      <c r="BE11" s="3"/>
+      <c r="BF11" s="3"/>
+      <c r="BG11" s="3"/>
+      <c r="BH11" s="3"/>
+      <c r="BI11" s="3"/>
+      <c r="BJ11" s="3"/>
+      <c r="BK11" s="3"/>
+      <c r="BL11" s="3"/>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="13"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="3"/>
+      <c r="BD12" s="3"/>
+      <c r="BE12" s="3"/>
+      <c r="BF12" s="3"/>
+      <c r="BG12" s="3"/>
+      <c r="BH12" s="3"/>
+      <c r="BI12" s="3"/>
+      <c r="BJ12" s="3"/>
+      <c r="BK12" s="3"/>
+      <c r="BL12" s="3"/>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="13"/>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+      <c r="BA13" s="1"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3"/>
+      <c r="BG13" s="3"/>
+      <c r="BH13" s="3"/>
+      <c r="BI13" s="3"/>
+      <c r="BJ13" s="3"/>
+      <c r="BK13" s="3"/>
+      <c r="BL13" s="3"/>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH14" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="11"/>
+      <c r="AO14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="13"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="2"/>
+      <c r="BC14" s="3"/>
+      <c r="BD14" s="3"/>
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
+      <c r="BI14" s="3"/>
+      <c r="BJ14" s="3"/>
+      <c r="BK14" s="3"/>
+      <c r="BL14" s="3"/>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="13"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="3"/>
+      <c r="BD15" s="3"/>
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3"/>
+      <c r="BG15" s="3"/>
+      <c r="BH15" s="3"/>
+      <c r="BI15" s="3"/>
+      <c r="BJ15" s="3"/>
+      <c r="BK15" s="3"/>
+      <c r="BL15" s="3"/>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="9"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="1"/>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="13"/>
+      <c r="AY16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AZ16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC16" s="3"/>
+      <c r="BD16" s="3"/>
+      <c r="BE16" s="3"/>
+      <c r="BF16" s="3"/>
+      <c r="BG16" s="3"/>
+      <c r="BH16" s="3"/>
+      <c r="BI16" s="3"/>
+      <c r="BJ16" s="3"/>
+      <c r="BK16" s="3"/>
+      <c r="BL16" s="3"/>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="9"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="AY17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AZ17" s="1"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="3"/>
+      <c r="BD17" s="3"/>
+      <c r="BE17" s="3"/>
+      <c r="BF17" s="3"/>
+      <c r="BG17" s="3"/>
+      <c r="BH17" s="3"/>
+      <c r="BI17" s="3"/>
+      <c r="BJ17" s="3"/>
+      <c r="BK17" s="3"/>
+      <c r="BL17" s="3"/>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1"/>
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AX18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="1"/>
+      <c r="BA18" s="1"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="3"/>
+      <c r="BD18" s="3"/>
+      <c r="BE18" s="3"/>
+      <c r="BF18" s="3"/>
+      <c r="BG18" s="3"/>
+      <c r="BH18" s="3"/>
+      <c r="BI18" s="3"/>
+      <c r="BJ18" s="3"/>
+      <c r="BK18" s="3"/>
+      <c r="BL18" s="3"/>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="1"/>
+      <c r="AS19" s="1"/>
+      <c r="AV19" t="s">
+        <v>5</v>
+      </c>
+      <c r="AW19" t="s">
+        <v>4</v>
+      </c>
+      <c r="BC19" s="3"/>
+      <c r="BD19" s="3"/>
+      <c r="BE19" s="3"/>
+      <c r="BF19" s="3"/>
+      <c r="BG19" s="3"/>
+      <c r="BH19" s="3"/>
+      <c r="BI19" s="3"/>
+      <c r="BJ19" s="3"/>
+      <c r="BK19" s="3"/>
+      <c r="BL19" s="3"/>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="1"/>
+      <c r="AM20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN20" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AO20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AT20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AU20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW20" s="1"/>
+      <c r="AX20" s="13"/>
+      <c r="AY20" s="1"/>
+      <c r="AZ20" s="1"/>
+      <c r="BA20" s="1"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="3"/>
+      <c r="BD20" s="3"/>
+      <c r="BE20" s="3"/>
+      <c r="BF20" s="3"/>
+      <c r="BG20" s="3"/>
+      <c r="BH20" s="3"/>
+      <c r="BI20" s="3"/>
+      <c r="BJ20" s="3"/>
+      <c r="BK20" s="3"/>
+      <c r="BL20" s="3"/>
+    </row>
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO21" s="1"/>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="1"/>
+      <c r="AR21" s="1"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="1"/>
+      <c r="AX21" s="13"/>
+      <c r="AY21" s="1"/>
+      <c r="AZ21" s="1"/>
+      <c r="BA21" s="1"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="3"/>
+      <c r="BD21" s="3"/>
+      <c r="BE21" s="3"/>
+      <c r="BF21" s="3"/>
+      <c r="BG21" s="3"/>
+      <c r="BH21" s="3"/>
+      <c r="BI21" s="3"/>
+      <c r="BJ21" s="3"/>
+      <c r="BK21" s="3"/>
+      <c r="BL21" s="3"/>
+    </row>
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="1"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
+      <c r="AR22" s="1"/>
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1"/>
+      <c r="AU22" s="1"/>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="13"/>
+      <c r="AY22" s="1"/>
+      <c r="AZ22" s="1"/>
+      <c r="BA22" s="1"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="3"/>
+      <c r="BD22" s="3"/>
+      <c r="BE22" s="3"/>
+      <c r="BF22" s="3"/>
+      <c r="BG22" s="3"/>
+      <c r="BH22" s="3"/>
+      <c r="BI22" s="3"/>
+      <c r="BJ22" s="3"/>
+      <c r="BK22" s="3"/>
+      <c r="BL22" s="3"/>
+    </row>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="1"/>
+      <c r="AL23" s="1"/>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="11"/>
+      <c r="AO23" s="1"/>
+      <c r="AP23" s="1"/>
+      <c r="AQ23" s="1"/>
+      <c r="AR23" s="1"/>
+      <c r="AS23" s="1"/>
+      <c r="AT23" s="1"/>
+      <c r="AU23" s="1"/>
+      <c r="AV23" s="1"/>
+      <c r="AW23" s="1"/>
+      <c r="AX23" s="13"/>
+      <c r="AY23" s="1"/>
+      <c r="AZ23" s="1"/>
+      <c r="BA23" s="1"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="3"/>
+      <c r="BD23" s="3"/>
+      <c r="BE23" s="3"/>
+      <c r="BF23" s="3"/>
+      <c r="BG23" s="3"/>
+      <c r="BH23" s="3"/>
+      <c r="BI23" s="3"/>
+      <c r="BJ23" s="3"/>
+      <c r="BK23" s="3"/>
+      <c r="BL23" s="3"/>
+    </row>
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="11"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="1"/>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1"/>
+      <c r="AU24" s="1"/>
+      <c r="AV24" s="1"/>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="13"/>
+      <c r="AY24" s="1"/>
+      <c r="AZ24" s="1"/>
+      <c r="BA24" s="1"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="3"/>
+      <c r="BD24" s="3"/>
+      <c r="BE24" s="3"/>
+      <c r="BF24" s="3"/>
+      <c r="BG24" s="3"/>
+      <c r="BH24" s="3"/>
+      <c r="BI24" s="3"/>
+      <c r="BJ24" s="3"/>
+      <c r="BK24" s="3"/>
+      <c r="BL24" s="3"/>
+    </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="11"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="1"/>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1"/>
+      <c r="AU25" s="1"/>
+      <c r="AV25" s="1"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="13"/>
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="1"/>
+      <c r="BA25" s="1"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="3"/>
+      <c r="BD25" s="3"/>
+      <c r="BE25" s="3"/>
+      <c r="BF25" s="3"/>
+      <c r="BG25" s="3"/>
+      <c r="BH25" s="3"/>
+      <c r="BI25" s="3"/>
+      <c r="BJ25" s="3"/>
+      <c r="BK25" s="3"/>
+      <c r="BL25" s="3"/>
+    </row>
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="1"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="11"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="1"/>
+      <c r="AS26" s="1"/>
+      <c r="AT26" s="1"/>
+      <c r="AU26" s="1"/>
+      <c r="AV26" s="1"/>
+      <c r="AW26" s="1"/>
+      <c r="AX26" s="13"/>
+      <c r="AY26" s="1"/>
+      <c r="AZ26" s="1"/>
+      <c r="BA26" s="1"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="3"/>
+      <c r="BD26" s="3"/>
+      <c r="BE26" s="3"/>
+      <c r="BF26" s="3"/>
+      <c r="BG26" s="3"/>
+      <c r="BH26" s="3"/>
+      <c r="BI26" s="3"/>
+      <c r="BJ26" s="3"/>
+      <c r="BK26" s="3"/>
+      <c r="BL26" s="3"/>
+    </row>
+    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="11"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="1"/>
+      <c r="AR27" s="1"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="1"/>
+      <c r="AY27" s="1"/>
+      <c r="AZ27" s="1"/>
+      <c r="BA27" s="1"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="3"/>
+      <c r="BD27" s="3"/>
+      <c r="BE27" s="3"/>
+      <c r="BF27" s="3"/>
+      <c r="BG27" s="3"/>
+      <c r="BH27" s="3"/>
+      <c r="BI27" s="3"/>
+      <c r="BJ27" s="3"/>
+      <c r="BK27" s="3"/>
+      <c r="BL27" s="3"/>
+    </row>
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="11"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="13"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1"/>
+      <c r="BA28" s="1"/>
+      <c r="BB28" s="2"/>
+      <c r="BC28" s="3"/>
+      <c r="BD28" s="3"/>
+      <c r="BE28" s="3"/>
+      <c r="BF28" s="3"/>
+      <c r="BG28" s="3"/>
+      <c r="BH28" s="3"/>
+      <c r="BI28" s="3"/>
+      <c r="BJ28" s="3"/>
+      <c r="BK28" s="3"/>
+      <c r="BL28" s="3"/>
+    </row>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="11"/>
+      <c r="AO29" s="1"/>
+      <c r="AP29" s="1"/>
+      <c r="AQ29" s="1"/>
+      <c r="AR29" s="1"/>
+      <c r="AS29" s="1"/>
+      <c r="AT29" s="1"/>
+      <c r="AU29" s="1"/>
+      <c r="AV29" s="1"/>
+      <c r="AW29" s="1"/>
+      <c r="AX29" s="13"/>
+      <c r="AY29" s="1"/>
+      <c r="AZ29" s="1"/>
+      <c r="BA29" s="1"/>
+      <c r="BB29" s="2"/>
+      <c r="BC29" s="3"/>
+      <c r="BD29" s="3"/>
+      <c r="BE29" s="3"/>
+      <c r="BF29" s="3"/>
+      <c r="BG29" s="3"/>
+      <c r="BH29" s="3"/>
+      <c r="BI29" s="3"/>
+      <c r="BJ29" s="3"/>
+      <c r="BK29" s="3"/>
+      <c r="BL29" s="3"/>
+    </row>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="15"/>
+      <c r="AC30" s="15"/>
+      <c r="AD30" s="18"/>
+      <c r="AE30" s="15"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="15"/>
+      <c r="AH30" s="15"/>
+      <c r="AI30" s="15"/>
+      <c r="AJ30" s="15"/>
+      <c r="AK30" s="15"/>
+      <c r="AL30" s="15"/>
+      <c r="AM30" s="15"/>
+      <c r="AN30" s="22"/>
+      <c r="AO30" s="15"/>
+      <c r="AP30" s="15"/>
+      <c r="AQ30" s="15"/>
+      <c r="AR30" s="15"/>
+      <c r="AS30" s="15"/>
+      <c r="AT30" s="15"/>
+      <c r="AU30" s="15"/>
+      <c r="AV30" s="15"/>
+      <c r="AW30" s="15"/>
+      <c r="AX30" s="23"/>
+      <c r="AY30" s="15"/>
+      <c r="AZ30" s="15"/>
+      <c r="BA30" s="15"/>
+      <c r="BB30" s="24"/>
+      <c r="BC30" s="3"/>
+      <c r="BD30" s="3"/>
+      <c r="BE30" s="3"/>
+      <c r="BF30" s="3"/>
+      <c r="BG30" s="3"/>
+      <c r="BH30" s="3"/>
+      <c r="BI30" s="3"/>
+      <c r="BJ30" s="3"/>
+      <c r="BK30" s="3"/>
+      <c r="BL30" s="3"/>
+    </row>
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="21"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
+      <c r="AN31" s="25"/>
+      <c r="AO31" s="3"/>
+      <c r="AP31" s="3"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="3"/>
+      <c r="AU31" s="3"/>
+      <c r="AV31" s="3"/>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="26"/>
+      <c r="AY31" s="3"/>
+      <c r="AZ31" s="3"/>
+      <c r="BA31" s="3"/>
+      <c r="BB31" s="3"/>
+      <c r="BC31" s="3"/>
+      <c r="BD31" s="3"/>
+      <c r="BE31" s="3"/>
+      <c r="BF31" s="3"/>
+      <c r="BG31" s="3"/>
+      <c r="BH31" s="3"/>
+      <c r="BI31" s="3"/>
+      <c r="BJ31" s="3"/>
+      <c r="BK31" s="3"/>
+      <c r="BL31" s="3"/>
+    </row>
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
+      <c r="AM32" s="3"/>
+      <c r="AN32" s="25"/>
+      <c r="AO32" s="3"/>
+      <c r="AP32" s="3"/>
+      <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
+      <c r="AS32" s="3"/>
+      <c r="AT32" s="3"/>
+      <c r="AU32" s="3"/>
+      <c r="AV32" s="3"/>
+      <c r="AW32" s="3"/>
+      <c r="AX32" s="26"/>
+      <c r="AY32" s="3"/>
+      <c r="AZ32" s="3"/>
+      <c r="BA32" s="3"/>
+      <c r="BB32" s="3"/>
+      <c r="BC32" s="3"/>
+      <c r="BD32" s="3"/>
+      <c r="BE32" s="3"/>
+      <c r="BF32" s="3"/>
+      <c r="BG32" s="3"/>
+      <c r="BH32" s="3"/>
+      <c r="BI32" s="3"/>
+      <c r="BJ32" s="3"/>
+      <c r="BK32" s="3"/>
+      <c r="BL32" s="3"/>
+    </row>
+    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="21"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="3"/>
+      <c r="AM33" s="3"/>
+      <c r="AN33" s="25"/>
+      <c r="AO33" s="3"/>
+      <c r="AP33" s="3"/>
+      <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
+      <c r="AS33" s="3"/>
+      <c r="AT33" s="3"/>
+      <c r="AU33" s="3"/>
+      <c r="AV33" s="3"/>
+      <c r="AW33" s="3"/>
+      <c r="AX33" s="26"/>
+      <c r="AY33" s="3"/>
+      <c r="AZ33" s="3"/>
+      <c r="BA33" s="3"/>
+      <c r="BB33" s="3"/>
+      <c r="BC33" s="3"/>
+      <c r="BD33" s="3"/>
+      <c r="BE33" s="3"/>
+      <c r="BF33" s="3"/>
+      <c r="BG33" s="3"/>
+      <c r="BH33" s="3"/>
+      <c r="BI33" s="3"/>
+      <c r="BJ33" s="3"/>
+      <c r="BK33" s="3"/>
+      <c r="BL33" s="3"/>
+    </row>
+    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="21"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3"/>
+      <c r="AL34" s="3"/>
+      <c r="AM34" s="3"/>
+      <c r="AN34" s="25"/>
+      <c r="AO34" s="3"/>
+      <c r="AP34" s="3"/>
+      <c r="AQ34" s="3"/>
+      <c r="AR34" s="3"/>
+      <c r="AS34" s="3"/>
+      <c r="AT34" s="3"/>
+      <c r="AU34" s="3"/>
+      <c r="AV34" s="3"/>
+      <c r="AW34" s="3"/>
+      <c r="AX34" s="26"/>
+      <c r="AY34" s="3"/>
+      <c r="AZ34" s="3"/>
+      <c r="BA34" s="3"/>
+      <c r="BB34" s="3"/>
+      <c r="BC34" s="3"/>
+      <c r="BD34" s="3"/>
+      <c r="BE34" s="3"/>
+      <c r="BF34" s="3"/>
+      <c r="BG34" s="3"/>
+      <c r="BH34" s="3"/>
+      <c r="BI34" s="3"/>
+      <c r="BJ34" s="3"/>
+      <c r="BK34" s="3"/>
+      <c r="BL34" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
responzive map next previous player chest home element added base map resize not work
</commit_message>
<xml_diff>
--- a/GUI_20212202_AYZ8R9/Maps/map.xlsx
+++ b/GUI_20212202_AYZ8R9/Maps/map.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\game\GUI_20212202_AYZ8R9\Maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\game3\GUI_20212202_AYZ8R9\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490DD743-0C61-4062-A791-0F25EC80B570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409971BD-C55B-411D-8B15-D553E955361D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Munka1" sheetId="1" r:id="rId1"/>
+    <sheet name="Munka1" sheetId="4" r:id="rId1"/>
     <sheet name="Munka2" sheetId="2" r:id="rId2"/>
     <sheet name="Munka3" sheetId="3" r:id="rId3"/>
+    <sheet name="Munka4" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="16">
   <si>
     <t>B</t>
   </si>
@@ -67,6 +68,24 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>NEXT</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>CHEST</t>
+  </si>
+  <si>
+    <t>PLAYER</t>
+  </si>
+  <si>
+    <t>HOME</t>
   </si>
 </sst>
 </file>
@@ -503,11 +522,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382D7427-FBDE-4BF3-ADAB-21A4C37623DD}">
+  <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AS37" sqref="AS37"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,10 +1084,6 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="7"/>
-      <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
@@ -1131,10 +1146,6 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-      <c r="R10" s="1"/>
-      <c r="S10" s="1"/>
-      <c r="T10" s="7"/>
-      <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
@@ -1197,10 +1208,6 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-      <c r="R11" s="1"/>
-      <c r="S11" s="1"/>
-      <c r="T11" s="7"/>
-      <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
@@ -1263,10 +1270,6 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-      <c r="R12" s="1"/>
-      <c r="S12" s="1"/>
-      <c r="T12" s="7"/>
-      <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
@@ -1329,10 +1332,6 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-      <c r="R13" s="1"/>
-      <c r="S13" s="1"/>
-      <c r="T13" s="7"/>
-      <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
@@ -1340,42 +1339,18 @@
       <c r="Z13" s="1"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
-      <c r="AC13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="AE13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="AC13" s="1"/>
+      <c r="AD13" s="9"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AJ13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+      <c r="AN13" s="11"/>
       <c r="AO13" s="1"/>
       <c r="AP13" s="1"/>
       <c r="AQ13" s="1"/>
@@ -1402,7 +1377,6 @@
       <c r="BL13" s="3"/>
     </row>
     <row r="14" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -1419,23 +1393,26 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-      <c r="R14" s="1"/>
-      <c r="S14" s="1"/>
-      <c r="T14" s="7"/>
-      <c r="U14" s="1"/>
+      <c r="R14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U14" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
-      <c r="AC14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD14" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="9"/>
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
@@ -1445,12 +1422,8 @@
       <c r="AK14" s="1"/>
       <c r="AL14" s="1"/>
       <c r="AM14" s="1"/>
-      <c r="AN14" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO14" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AN14" s="11"/>
+      <c r="AO14" s="1"/>
       <c r="AP14" s="1"/>
       <c r="AQ14" s="1"/>
       <c r="AR14" s="1"/>
@@ -1463,7 +1436,6 @@
       <c r="AY14" s="1"/>
       <c r="AZ14" s="1"/>
       <c r="BA14" s="1"/>
-      <c r="BB14" s="2"/>
       <c r="BC14" s="3"/>
       <c r="BD14" s="3"/>
       <c r="BE14" s="3"/>
@@ -1476,101 +1448,27 @@
       <c r="BL14" s="3"/>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
-      <c r="Q15" s="1"/>
-      <c r="R15" s="1"/>
-      <c r="S15" s="1"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD15" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
-      <c r="AG15" s="1"/>
-      <c r="AH15" s="1"/>
-      <c r="AI15" s="1"/>
-      <c r="AJ15" s="1"/>
-      <c r="AK15" s="1"/>
-      <c r="AL15" s="1"/>
-      <c r="AM15" s="1"/>
-      <c r="AN15" s="11"/>
-      <c r="AO15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AQ15" s="1"/>
-      <c r="AR15" s="1"/>
-      <c r="AS15" s="1"/>
-      <c r="AT15" s="1"/>
-      <c r="AU15" s="1"/>
-      <c r="AV15" s="1"/>
-      <c r="AW15" s="1"/>
-      <c r="AX15" s="13"/>
-      <c r="AY15" s="1"/>
-      <c r="AZ15" s="1"/>
-      <c r="BA15" s="1"/>
-      <c r="BB15" s="2"/>
-      <c r="BC15" s="3"/>
-      <c r="BD15" s="3"/>
-      <c r="BE15" s="3"/>
-      <c r="BF15" s="3"/>
-      <c r="BG15" s="3"/>
-      <c r="BH15" s="3"/>
-      <c r="BI15" s="3"/>
-      <c r="BJ15" s="3"/>
-      <c r="BK15" s="3"/>
-      <c r="BL15" s="3"/>
+      <c r="R15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U15" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="5"/>
@@ -1581,10 +1479,18 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-      <c r="R16" s="1"/>
-      <c r="S16" s="1"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="1"/>
+      <c r="R16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
       <c r="X16" s="1"/>
@@ -1592,12 +1498,8 @@
       <c r="Z16" s="1"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
-      <c r="AC16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD16" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="9"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
@@ -1609,12 +1511,8 @@
       <c r="AM16" s="1"/>
       <c r="AN16" s="11"/>
       <c r="AO16" s="1"/>
-      <c r="AP16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ16" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AP16" s="1"/>
+      <c r="AQ16" s="1"/>
       <c r="AR16" s="1"/>
       <c r="AS16" s="1"/>
       <c r="AT16" s="1"/>
@@ -1638,16 +1536,13 @@
       <c r="BL16" s="3"/>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="5"/>
       <c r="K17" s="1"/>
@@ -1657,23 +1552,26 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="1"/>
-      <c r="S17" s="1"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="1"/>
+      <c r="R17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
       <c r="Y17" s="1"/>
       <c r="Z17" s="1"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
-      <c r="AC17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD17" s="9" t="s">
-        <v>6</v>
-      </c>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="9"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
@@ -1686,12 +1584,8 @@
       <c r="AN17" s="11"/>
       <c r="AO17" s="1"/>
       <c r="AP17" s="1"/>
-      <c r="AQ17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR17" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="1"/>
       <c r="AS17" s="1"/>
       <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
@@ -1714,103 +1608,23 @@
       <c r="BL17" s="3"/>
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="P18" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="R18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S18" s="1"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD18" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
-      <c r="AG18" s="1"/>
-      <c r="AH18" s="1"/>
-      <c r="AI18" s="1"/>
-      <c r="AJ18" s="1"/>
-      <c r="AK18" s="1"/>
-      <c r="AL18" s="1"/>
-      <c r="AM18" s="1"/>
-      <c r="AN18" s="11"/>
-      <c r="AO18" s="1"/>
-      <c r="AP18" s="1"/>
-      <c r="AQ18" s="1"/>
-      <c r="AR18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AT18" s="1"/>
-      <c r="AU18" s="1"/>
-      <c r="AV18" s="1"/>
-      <c r="AW18" s="1"/>
-      <c r="AX18" s="13"/>
-      <c r="AY18" s="1"/>
-      <c r="AZ18" s="1"/>
-      <c r="BA18" s="1"/>
-      <c r="BB18" s="2"/>
-      <c r="BC18" s="3"/>
-      <c r="BD18" s="3"/>
-      <c r="BE18" s="3"/>
-      <c r="BF18" s="3"/>
-      <c r="BG18" s="3"/>
-      <c r="BH18" s="3"/>
-      <c r="BI18" s="3"/>
-      <c r="BJ18" s="3"/>
-      <c r="BK18" s="3"/>
-      <c r="BL18" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -1826,28 +1640,30 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-      <c r="Q19" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="Q19" s="1"/>
       <c r="R19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S19" s="1"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="1"/>
+        <v>15</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="V19" s="1"/>
       <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
+      <c r="X19" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
-      <c r="AC19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AD19" s="9" t="s">
-        <v>4</v>
-      </c>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="9"/>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
@@ -1862,11 +1678,9 @@
       <c r="AP19" s="1"/>
       <c r="AQ19" s="1"/>
       <c r="AR19" s="1"/>
-      <c r="AS19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT19" t="s">
-        <v>2</v>
+      <c r="AS19" s="1"/>
+      <c r="BB19" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="BC19" s="3"/>
       <c r="BD19" s="3"/>
@@ -1880,61 +1694,143 @@
       <c r="BL19" s="3"/>
     </row>
     <row r="20" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="Q20" s="1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="S20" s="1"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="S20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AB20" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AC20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD20" s="9"/>
-      <c r="AE20" s="1"/>
-      <c r="AF20" s="1"/>
-      <c r="AG20" s="1"/>
-      <c r="AH20" s="1"/>
-      <c r="AI20" s="1"/>
-      <c r="AJ20" s="1"/>
-      <c r="AK20" s="1"/>
-      <c r="AL20" s="1"/>
-      <c r="AM20" s="1"/>
-      <c r="AN20" s="11"/>
-      <c r="AO20" s="1"/>
-      <c r="AP20" s="1"/>
-      <c r="AQ20" s="1"/>
-      <c r="AR20" s="1"/>
-      <c r="AS20" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AP20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AR20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AS20" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="AT20" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU20" s="1" t="s">
         <v>0</v>
@@ -1945,7 +1841,7 @@
       <c r="AW20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AX20" s="13" t="s">
+      <c r="AX20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AY20" s="1" t="s">
@@ -1957,7 +1853,7 @@
       <c r="BA20" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="BB20" s="2" t="s">
+      <c r="BB20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="BC20" s="3"/>
@@ -1988,12 +1884,8 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-      <c r="Q21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R21" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="7"/>
       <c r="U21" s="1"/>
@@ -2002,12 +1894,8 @@
       <c r="X21" s="1"/>
       <c r="Y21" s="1"/>
       <c r="Z21" s="1"/>
-      <c r="AA21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB21" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
       <c r="AD21" s="9"/>
       <c r="AE21" s="1"/>
@@ -2062,12 +1950,8 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-      <c r="Q22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="7"/>
       <c r="U22" s="1"/>
@@ -2075,12 +1959,8 @@
       <c r="W22" s="1"/>
       <c r="X22" s="1"/>
       <c r="Y22" s="1"/>
-      <c r="Z22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA22" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
       <c r="AB22" s="1"/>
       <c r="AC22" s="1"/>
       <c r="AD22" s="9"/>
@@ -2136,24 +2016,16 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-      <c r="Q23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="7"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
-      <c r="Y23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z23" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
       <c r="AA23" s="1"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
@@ -2210,33 +2082,15 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="S24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="T24" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="U24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
       <c r="Z24" s="1"/>
       <c r="AA24" s="1"/>
       <c r="AB24" s="1"/>
@@ -2936,19 +2790,8 @@
       <c r="BK34" s="3"/>
       <c r="BL34" s="3"/>
     </row>
-    <row r="36" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="AT36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="AU39" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2956,8 +2799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32EA023-0038-482A-B633-0391C0CB8525}">
   <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AW23" sqref="AW23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4154,7 +3997,7 @@
         <v>9</v>
       </c>
       <c r="BB15" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="BC15" s="3"/>
       <c r="BD15" s="3"/>
@@ -4428,7 +4271,9 @@
         <v>2</v>
       </c>
       <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
+      <c r="S18" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="T18" s="7" t="s">
         <v>5</v>
       </c>
@@ -4508,7 +4353,9 @@
       <c r="BL18" s="3"/>
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -4532,7 +4379,9 @@
         <v>3</v>
       </c>
       <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
+      <c r="S19" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="T19" s="7" t="s">
         <v>6</v>
       </c>
@@ -4631,7 +4480,9 @@
         <v>3</v>
       </c>
       <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
+      <c r="S20" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="T20" s="7" t="s">
         <v>6</v>
       </c>
@@ -4721,7 +4572,9 @@
         <v>3</v>
       </c>
       <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
+      <c r="S21" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="T21" s="7" t="s">
         <v>6</v>
       </c>
@@ -4791,7 +4644,9 @@
         <v>3</v>
       </c>
       <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
+      <c r="S22" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="T22" s="7" t="s">
         <v>6</v>
       </c>
@@ -4861,7 +4716,9 @@
         <v>3</v>
       </c>
       <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
+      <c r="S23" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="T23" s="7" t="s">
         <v>6</v>
       </c>
@@ -4931,7 +4788,9 @@
         <v>3</v>
       </c>
       <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
+      <c r="S24" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="T24" s="7" t="s">
         <v>6</v>
       </c>
@@ -5000,8 +4859,12 @@
       <c r="Q25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
+      <c r="R25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="T25" s="7" t="s">
         <v>6</v>
       </c>
@@ -5660,8 +5523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8F6284-F138-4CEB-A50F-8C3CA6F27EB7}">
   <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AM16" sqref="AM16"/>
+    <sheetView topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX13" sqref="AX13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6448,7 +6311,9 @@
       <c r="AX10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="AY10" s="1"/>
+      <c r="AY10" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="AZ10" s="1"/>
       <c r="BA10" s="1"/>
       <c r="BB10" s="2"/>
@@ -6629,7 +6494,9 @@
         <v>2</v>
       </c>
       <c r="BA12" s="1"/>
-      <c r="BB12" s="2"/>
+      <c r="BB12" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="BC12" s="3"/>
       <c r="BD12" s="3"/>
       <c r="BE12" s="3"/>
@@ -6816,7 +6683,9 @@
       <c r="BL14" s="3"/>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1" t="s">
@@ -7624,7 +7493,9 @@
       </c>
       <c r="W25" s="1"/>
       <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
+      <c r="Y25" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="Z25" s="1"/>
       <c r="AA25" s="1"/>
       <c r="AB25" s="1"/>
@@ -8293,4 +8164,2468 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BL39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="9.140625" style="6"/>
+    <col min="20" max="20" width="9.140625" style="8"/>
+    <col min="30" max="30" width="9.140625" style="10"/>
+    <col min="40" max="40" width="9.140625" style="12"/>
+    <col min="50" max="50" width="9.140625" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
+      <c r="AX1" s="13"/>
+      <c r="AY1" s="1"/>
+      <c r="AZ1" s="1"/>
+      <c r="BA1" s="1"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
+      <c r="BE1" s="3"/>
+      <c r="BF1" s="3"/>
+      <c r="BG1" s="3"/>
+      <c r="BH1" s="3"/>
+      <c r="BI1" s="3"/>
+      <c r="BJ1" s="3"/>
+      <c r="BK1" s="3"/>
+      <c r="BL1" s="3"/>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="9"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
+      <c r="AI2" s="1"/>
+      <c r="AJ2" s="1"/>
+      <c r="AK2" s="1"/>
+      <c r="AL2" s="1"/>
+      <c r="AM2" s="1"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="1"/>
+      <c r="AP2" s="1"/>
+      <c r="AQ2" s="1"/>
+      <c r="AR2" s="1"/>
+      <c r="AS2" s="1"/>
+      <c r="AT2" s="1"/>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" s="1"/>
+      <c r="AX2" s="13"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" s="1"/>
+      <c r="BA2" s="1"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="3"/>
+      <c r="BD2" s="3"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="3"/>
+      <c r="BH2" s="3"/>
+      <c r="BI2" s="3"/>
+      <c r="BJ2" s="3"/>
+      <c r="BK2" s="3"/>
+      <c r="BL2" s="3"/>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
+      <c r="AK3" s="1"/>
+      <c r="AL3" s="1"/>
+      <c r="AM3" s="1"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="1"/>
+      <c r="AP3" s="1"/>
+      <c r="AQ3" s="1"/>
+      <c r="AR3" s="1"/>
+      <c r="AS3" s="1"/>
+      <c r="AT3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
+      <c r="AW3" s="1"/>
+      <c r="AX3" s="13"/>
+      <c r="AY3" s="1"/>
+      <c r="AZ3" s="1"/>
+      <c r="BA3" s="1"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3"/>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
+      <c r="BI3" s="3"/>
+      <c r="BJ3" s="3"/>
+      <c r="BK3" s="3"/>
+      <c r="BL3" s="3"/>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+      <c r="AB4" s="1"/>
+      <c r="AC4" s="1"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="1"/>
+      <c r="AF4" s="1"/>
+      <c r="AG4" s="1"/>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1"/>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1"/>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="1"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="1"/>
+      <c r="AP4" s="1"/>
+      <c r="AQ4" s="1"/>
+      <c r="AR4" s="1"/>
+      <c r="AS4" s="1"/>
+      <c r="AT4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
+      <c r="AW4" s="1"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="1"/>
+      <c r="AZ4" s="1"/>
+      <c r="BA4" s="1"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="3"/>
+      <c r="BD4" s="3"/>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3"/>
+      <c r="BG4" s="3"/>
+      <c r="BH4" s="3"/>
+      <c r="BI4" s="3"/>
+      <c r="BJ4" s="3"/>
+      <c r="BK4" s="3"/>
+      <c r="BL4" s="3"/>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
+      <c r="AH5" s="1"/>
+      <c r="AI5" s="1"/>
+      <c r="AJ5" s="1"/>
+      <c r="AK5" s="1"/>
+      <c r="AL5" s="1"/>
+      <c r="AM5" s="1"/>
+      <c r="AN5" s="11"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
+      <c r="AQ5" s="1"/>
+      <c r="AR5" s="1"/>
+      <c r="AS5" s="1"/>
+      <c r="AT5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
+      <c r="AW5" s="1"/>
+      <c r="AX5" s="13"/>
+      <c r="AY5" s="1"/>
+      <c r="AZ5" s="1"/>
+      <c r="BA5" s="1"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="3"/>
+      <c r="BD5" s="3"/>
+      <c r="BE5" s="3"/>
+      <c r="BF5" s="3"/>
+      <c r="BG5" s="3"/>
+      <c r="BH5" s="3"/>
+      <c r="BI5" s="3"/>
+      <c r="BJ5" s="3"/>
+      <c r="BK5" s="3"/>
+      <c r="BL5" s="3"/>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="11"/>
+      <c r="AO6" s="1"/>
+      <c r="AP6" s="1"/>
+      <c r="AQ6" s="1"/>
+      <c r="AR6" s="1"/>
+      <c r="AS6" s="1"/>
+      <c r="AT6" s="1"/>
+      <c r="AU6" s="1"/>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="1"/>
+      <c r="AX6" s="13"/>
+      <c r="AY6" s="1"/>
+      <c r="AZ6" s="1"/>
+      <c r="BA6" s="1"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="3"/>
+      <c r="BD6" s="3"/>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3"/>
+      <c r="BG6" s="3"/>
+      <c r="BH6" s="3"/>
+      <c r="BI6" s="3"/>
+      <c r="BJ6" s="3"/>
+      <c r="BK6" s="3"/>
+      <c r="BL6" s="3"/>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="9"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AG7" s="1"/>
+      <c r="AH7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+      <c r="AK7" s="1"/>
+      <c r="AL7" s="1"/>
+      <c r="AM7" s="1"/>
+      <c r="AN7" s="11"/>
+      <c r="AO7" s="1"/>
+      <c r="AP7" s="1"/>
+      <c r="AQ7" s="1"/>
+      <c r="AR7" s="1"/>
+      <c r="AS7" s="1"/>
+      <c r="AT7" s="1"/>
+      <c r="AU7" s="1"/>
+      <c r="AV7" s="1"/>
+      <c r="AW7" s="1"/>
+      <c r="AX7" s="13"/>
+      <c r="AY7" s="1"/>
+      <c r="AZ7" s="1"/>
+      <c r="BA7" s="1"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="3"/>
+      <c r="BD7" s="3"/>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="3"/>
+      <c r="BH7" s="3"/>
+      <c r="BI7" s="3"/>
+      <c r="BJ7" s="3"/>
+      <c r="BK7" s="3"/>
+      <c r="BL7" s="3"/>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+      <c r="AB8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AD8" s="9"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+      <c r="AK8" s="1"/>
+      <c r="AL8" s="1"/>
+      <c r="AM8" s="1"/>
+      <c r="AN8" s="11"/>
+      <c r="AO8" s="1"/>
+      <c r="AP8" s="1"/>
+      <c r="AQ8" s="1"/>
+      <c r="AR8" s="1"/>
+      <c r="AS8" s="1"/>
+      <c r="AT8" s="1"/>
+      <c r="AU8" s="1"/>
+      <c r="AV8" s="1"/>
+      <c r="AW8" s="1"/>
+      <c r="AX8" s="13"/>
+      <c r="AY8" s="1"/>
+      <c r="AZ8" s="1"/>
+      <c r="BA8" s="1"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="3"/>
+      <c r="BD8" s="3"/>
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3"/>
+      <c r="BG8" s="3"/>
+      <c r="BH8" s="3"/>
+      <c r="BI8" s="3"/>
+      <c r="BJ8" s="3"/>
+      <c r="BK8" s="3"/>
+      <c r="BL8" s="3"/>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="9"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="11"/>
+      <c r="AO9" s="1"/>
+      <c r="AP9" s="1"/>
+      <c r="AQ9" s="1"/>
+      <c r="AR9" s="1"/>
+      <c r="AS9" s="1"/>
+      <c r="AT9" s="1"/>
+      <c r="AU9" s="1"/>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="1"/>
+      <c r="AX9" s="13"/>
+      <c r="AY9" s="1"/>
+      <c r="AZ9" s="1"/>
+      <c r="BA9" s="1"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="3"/>
+      <c r="BD9" s="3"/>
+      <c r="BE9" s="3"/>
+      <c r="BF9" s="3"/>
+      <c r="BG9" s="3"/>
+      <c r="BH9" s="3"/>
+      <c r="BI9" s="3"/>
+      <c r="BJ9" s="3"/>
+      <c r="BK9" s="3"/>
+      <c r="BL9" s="3"/>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AC10" s="1"/>
+      <c r="AD10" s="9"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AH10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AK10" s="1"/>
+      <c r="AL10" s="1"/>
+      <c r="AM10" s="1"/>
+      <c r="AN10" s="11"/>
+      <c r="AO10" s="1"/>
+      <c r="AP10" s="1"/>
+      <c r="AQ10" s="1"/>
+      <c r="AR10" s="1"/>
+      <c r="AS10" s="1"/>
+      <c r="AT10" s="1"/>
+      <c r="AU10" s="1"/>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="1"/>
+      <c r="AX10" s="13"/>
+      <c r="AY10" s="1"/>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="2"/>
+      <c r="BC10" s="3"/>
+      <c r="BD10" s="3"/>
+      <c r="BE10" s="3"/>
+      <c r="BF10" s="3"/>
+      <c r="BG10" s="3"/>
+      <c r="BH10" s="3"/>
+      <c r="BI10" s="3"/>
+      <c r="BJ10" s="3"/>
+      <c r="BK10" s="3"/>
+      <c r="BL10" s="3"/>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AD11" s="9"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AH11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="11"/>
+      <c r="AO11" s="1"/>
+      <c r="AP11" s="1"/>
+      <c r="AQ11" s="1"/>
+      <c r="AR11" s="1"/>
+      <c r="AS11" s="1"/>
+      <c r="AT11" s="1"/>
+      <c r="AU11" s="1"/>
+      <c r="AV11" s="1"/>
+      <c r="AW11" s="1"/>
+      <c r="AX11" s="13"/>
+      <c r="AY11" s="1"/>
+      <c r="AZ11" s="1"/>
+      <c r="BA11" s="1"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="3"/>
+      <c r="BD11" s="3"/>
+      <c r="BE11" s="3"/>
+      <c r="BF11" s="3"/>
+      <c r="BG11" s="3"/>
+      <c r="BH11" s="3"/>
+      <c r="BI11" s="3"/>
+      <c r="BJ11" s="3"/>
+      <c r="BK11" s="3"/>
+      <c r="BL11" s="3"/>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AL12" s="1"/>
+      <c r="AM12" s="1"/>
+      <c r="AN12" s="11"/>
+      <c r="AO12" s="1"/>
+      <c r="AP12" s="1"/>
+      <c r="AQ12" s="1"/>
+      <c r="AR12" s="1"/>
+      <c r="AS12" s="1"/>
+      <c r="AT12" s="1"/>
+      <c r="AU12" s="1"/>
+      <c r="AV12" s="1"/>
+      <c r="AW12" s="1"/>
+      <c r="AX12" s="13"/>
+      <c r="AY12" s="1"/>
+      <c r="AZ12" s="1"/>
+      <c r="BA12" s="1"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="3"/>
+      <c r="BD12" s="3"/>
+      <c r="BE12" s="3"/>
+      <c r="BF12" s="3"/>
+      <c r="BG12" s="3"/>
+      <c r="BH12" s="3"/>
+      <c r="BI12" s="3"/>
+      <c r="BJ12" s="3"/>
+      <c r="BK12" s="3"/>
+      <c r="BL12" s="3"/>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
+      <c r="AC13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AM13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="AO13" s="1"/>
+      <c r="AP13" s="1"/>
+      <c r="AQ13" s="1"/>
+      <c r="AR13" s="1"/>
+      <c r="AS13" s="1"/>
+      <c r="AT13" s="1"/>
+      <c r="AU13" s="1"/>
+      <c r="AV13" s="1"/>
+      <c r="AW13" s="1"/>
+      <c r="AX13" s="13"/>
+      <c r="AY13" s="1"/>
+      <c r="AZ13" s="1"/>
+      <c r="BA13" s="1"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="3"/>
+      <c r="BD13" s="3"/>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3"/>
+      <c r="BG13" s="3"/>
+      <c r="BH13" s="3"/>
+      <c r="BI13" s="3"/>
+      <c r="BJ13" s="3"/>
+      <c r="BK13" s="3"/>
+      <c r="BL13" s="3"/>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+      <c r="AG14" s="1"/>
+      <c r="AH14" s="1"/>
+      <c r="AI14" s="1"/>
+      <c r="AJ14" s="1"/>
+      <c r="AK14" s="1"/>
+      <c r="AL14" s="1"/>
+      <c r="AM14" s="1"/>
+      <c r="AN14" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO14" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AP14" s="1"/>
+      <c r="AQ14" s="1"/>
+      <c r="AR14" s="1"/>
+      <c r="AS14" s="1"/>
+      <c r="AT14" s="1"/>
+      <c r="AU14" s="1"/>
+      <c r="AV14" s="1"/>
+      <c r="AW14" s="1"/>
+      <c r="AX14" s="13"/>
+      <c r="AY14" s="1"/>
+      <c r="AZ14" s="1"/>
+      <c r="BA14" s="1"/>
+      <c r="BB14" s="2"/>
+      <c r="BC14" s="3"/>
+      <c r="BD14" s="3"/>
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
+      <c r="BI14" s="3"/>
+      <c r="BJ14" s="3"/>
+      <c r="BK14" s="3"/>
+      <c r="BL14" s="3"/>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AB15" s="1"/>
+      <c r="AC15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE15" s="1"/>
+      <c r="AF15" s="1"/>
+      <c r="AG15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AI15" s="1"/>
+      <c r="AJ15" s="1"/>
+      <c r="AK15" s="1"/>
+      <c r="AL15" s="1"/>
+      <c r="AM15" s="1"/>
+      <c r="AN15" s="11"/>
+      <c r="AO15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP15" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AQ15" s="1"/>
+      <c r="AR15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="1"/>
+      <c r="AU15" s="1"/>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="1"/>
+      <c r="AX15" s="13"/>
+      <c r="AY15" s="1"/>
+      <c r="AZ15" s="1"/>
+      <c r="BA15" s="1"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="3"/>
+      <c r="BD15" s="3"/>
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3"/>
+      <c r="BG15" s="3"/>
+      <c r="BH15" s="3"/>
+      <c r="BI15" s="3"/>
+      <c r="BJ15" s="3"/>
+      <c r="BK15" s="3"/>
+      <c r="BL15" s="3"/>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD16" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AH16" s="1"/>
+      <c r="AI16" s="1"/>
+      <c r="AJ16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AL16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="11"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AR16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="1"/>
+      <c r="AU16" s="1"/>
+      <c r="AV16" s="1"/>
+      <c r="AW16" s="1"/>
+      <c r="AX16" s="13"/>
+      <c r="AY16" s="1"/>
+      <c r="AZ16" s="1"/>
+      <c r="BA16" s="1"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="3"/>
+      <c r="BD16" s="3"/>
+      <c r="BE16" s="3"/>
+      <c r="BF16" s="3"/>
+      <c r="BG16" s="3"/>
+      <c r="BH16" s="3"/>
+      <c r="BI16" s="3"/>
+      <c r="BJ16" s="3"/>
+      <c r="BK16" s="3"/>
+      <c r="BL16" s="3"/>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" s="5"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD17" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AG17" s="1"/>
+      <c r="AH17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AJ17" s="1"/>
+      <c r="AK17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="11"/>
+      <c r="AO17" s="1"/>
+      <c r="AP17" s="1"/>
+      <c r="AQ17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="1"/>
+      <c r="AU17" s="1"/>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="1"/>
+      <c r="AX17" s="13"/>
+      <c r="AY17" s="1"/>
+      <c r="AZ17" s="1"/>
+      <c r="BA17" s="1"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="3"/>
+      <c r="BD17" s="3"/>
+      <c r="BE17" s="3"/>
+      <c r="BF17" s="3"/>
+      <c r="BG17" s="3"/>
+      <c r="BH17" s="3"/>
+      <c r="BI17" s="3"/>
+      <c r="BJ17" s="3"/>
+      <c r="BK17" s="3"/>
+      <c r="BL17" s="3"/>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S18" s="1"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="11"/>
+      <c r="AO18" s="1"/>
+      <c r="AP18" s="1"/>
+      <c r="AQ18" s="1"/>
+      <c r="AR18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AT18" s="1"/>
+      <c r="AU18" s="1"/>
+      <c r="AV18" s="1"/>
+      <c r="AW18" s="1"/>
+      <c r="AX18" s="13"/>
+      <c r="AY18" s="1"/>
+      <c r="AZ18" s="1"/>
+      <c r="BA18" s="1"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="3"/>
+      <c r="BD18" s="3"/>
+      <c r="BE18" s="3"/>
+      <c r="BF18" s="3"/>
+      <c r="BG18" s="3"/>
+      <c r="BH18" s="3"/>
+      <c r="BI18" s="3"/>
+      <c r="BJ18" s="3"/>
+      <c r="BK18" s="3"/>
+      <c r="BL18" s="3"/>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S19" s="1"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD19" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AG19" s="1"/>
+      <c r="AH19" s="1"/>
+      <c r="AI19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AK19" s="1"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="1"/>
+      <c r="AP19" s="1"/>
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="1"/>
+      <c r="AS19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT19" t="s">
+        <v>2</v>
+      </c>
+      <c r="BB19" t="s">
+        <v>12</v>
+      </c>
+      <c r="BC19" s="3"/>
+      <c r="BD19" s="3"/>
+      <c r="BE19" s="3"/>
+      <c r="BF19" s="3"/>
+      <c r="BG19" s="3"/>
+      <c r="BH19" s="3"/>
+      <c r="BI19" s="3"/>
+      <c r="BJ19" s="3"/>
+      <c r="BK19" s="3"/>
+      <c r="BL19" s="3"/>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD20" s="9"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AG20" s="1"/>
+      <c r="AH20" s="1"/>
+      <c r="AI20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AK20" s="1"/>
+      <c r="AL20" s="1"/>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="11"/>
+      <c r="AO20" s="1"/>
+      <c r="AP20" s="1"/>
+      <c r="AQ20" s="1"/>
+      <c r="AR20" s="1"/>
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AV20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AW20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AX20" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="AY20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AZ20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BA20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB20" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC20" s="3"/>
+      <c r="BD20" s="3"/>
+      <c r="BE20" s="3"/>
+      <c r="BF20" s="3"/>
+      <c r="BG20" s="3"/>
+      <c r="BH20" s="3"/>
+      <c r="BI20" s="3"/>
+      <c r="BJ20" s="3"/>
+      <c r="BK20" s="3"/>
+      <c r="BL20" s="3"/>
+    </row>
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S21" s="1"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+      <c r="AG21" s="1"/>
+      <c r="AH21" s="1"/>
+      <c r="AI21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AK21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="11"/>
+      <c r="AO21" s="1"/>
+      <c r="AP21" s="1"/>
+      <c r="AQ21" s="1"/>
+      <c r="AR21" s="1"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1"/>
+      <c r="AU21" s="1"/>
+      <c r="AV21" s="1"/>
+      <c r="AW21" s="1"/>
+      <c r="AX21" s="13"/>
+      <c r="AY21" s="1"/>
+      <c r="AZ21" s="1"/>
+      <c r="BA21" s="1"/>
+      <c r="BB21" s="2"/>
+      <c r="BC21" s="3"/>
+      <c r="BD21" s="3"/>
+      <c r="BE21" s="3"/>
+      <c r="BF21" s="3"/>
+      <c r="BG21" s="3"/>
+      <c r="BH21" s="3"/>
+      <c r="BI21" s="3"/>
+      <c r="BJ21" s="3"/>
+      <c r="BK21" s="3"/>
+      <c r="BL21" s="3"/>
+    </row>
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S22" s="1"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AK22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="11"/>
+      <c r="AO22" s="1"/>
+      <c r="AP22" s="1"/>
+      <c r="AQ22" s="1"/>
+      <c r="AR22" s="1"/>
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1"/>
+      <c r="AU22" s="1"/>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="13"/>
+      <c r="AY22" s="1"/>
+      <c r="AZ22" s="1"/>
+      <c r="BA22" s="1"/>
+      <c r="BB22" s="2"/>
+      <c r="BC22" s="3"/>
+      <c r="BD22" s="3"/>
+      <c r="BE22" s="3"/>
+      <c r="BF22" s="3"/>
+      <c r="BG22" s="3"/>
+      <c r="BH22" s="3"/>
+      <c r="BI22" s="3"/>
+      <c r="BJ22" s="3"/>
+      <c r="BK22" s="3"/>
+      <c r="BL22" s="3"/>
+    </row>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S23" s="1"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="9"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AG23" s="1"/>
+      <c r="AH23" s="1"/>
+      <c r="AI23" s="1"/>
+      <c r="AJ23" s="1"/>
+      <c r="AK23" s="1"/>
+      <c r="AL23" s="1"/>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="11"/>
+      <c r="AO23" s="1"/>
+      <c r="AP23" s="1"/>
+      <c r="AQ23" s="1"/>
+      <c r="AR23" s="1"/>
+      <c r="AS23" s="1"/>
+      <c r="AT23" s="1"/>
+      <c r="AU23" s="1"/>
+      <c r="AV23" s="1"/>
+      <c r="AW23" s="1"/>
+      <c r="AX23" s="13"/>
+      <c r="AY23" s="1"/>
+      <c r="AZ23" s="1"/>
+      <c r="BA23" s="1"/>
+      <c r="BB23" s="2"/>
+      <c r="BC23" s="3"/>
+      <c r="BD23" s="3"/>
+      <c r="BE23" s="3"/>
+      <c r="BF23" s="3"/>
+      <c r="BG23" s="3"/>
+      <c r="BH23" s="3"/>
+      <c r="BI23" s="3"/>
+      <c r="BJ23" s="3"/>
+      <c r="BK23" s="3"/>
+      <c r="BL23" s="3"/>
+    </row>
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AC24" s="1"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AJ24" s="1"/>
+      <c r="AK24" s="1"/>
+      <c r="AL24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="11"/>
+      <c r="AO24" s="1"/>
+      <c r="AP24" s="1"/>
+      <c r="AQ24" s="1"/>
+      <c r="AR24" s="1"/>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1"/>
+      <c r="AU24" s="1"/>
+      <c r="AV24" s="1"/>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="13"/>
+      <c r="AY24" s="1"/>
+      <c r="AZ24" s="1"/>
+      <c r="BA24" s="1"/>
+      <c r="BB24" s="2"/>
+      <c r="BC24" s="3"/>
+      <c r="BD24" s="3"/>
+      <c r="BE24" s="3"/>
+      <c r="BF24" s="3"/>
+      <c r="BG24" s="3"/>
+      <c r="BH24" s="3"/>
+      <c r="BI24" s="3"/>
+      <c r="BJ24" s="3"/>
+      <c r="BK24" s="3"/>
+      <c r="BL24" s="3"/>
+    </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+      <c r="AB25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="1"/>
+      <c r="AF25" s="1"/>
+      <c r="AG25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AI25" s="1"/>
+      <c r="AJ25" s="1"/>
+      <c r="AK25" s="1"/>
+      <c r="AL25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="11"/>
+      <c r="AO25" s="1"/>
+      <c r="AP25" s="1"/>
+      <c r="AQ25" s="1"/>
+      <c r="AR25" s="1"/>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1"/>
+      <c r="AU25" s="1"/>
+      <c r="AV25" s="1"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="13"/>
+      <c r="AY25" s="1"/>
+      <c r="AZ25" s="1"/>
+      <c r="BA25" s="1"/>
+      <c r="BB25" s="2"/>
+      <c r="BC25" s="3"/>
+      <c r="BD25" s="3"/>
+      <c r="BE25" s="3"/>
+      <c r="BF25" s="3"/>
+      <c r="BG25" s="3"/>
+      <c r="BH25" s="3"/>
+      <c r="BI25" s="3"/>
+      <c r="BJ25" s="3"/>
+      <c r="BK25" s="3"/>
+      <c r="BL25" s="3"/>
+    </row>
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+      <c r="AC26" s="1"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="1"/>
+      <c r="AF26" s="1"/>
+      <c r="AG26" s="1"/>
+      <c r="AH26" s="1"/>
+      <c r="AI26" s="1"/>
+      <c r="AJ26" s="1"/>
+      <c r="AK26" s="1"/>
+      <c r="AL26" s="1"/>
+      <c r="AM26" s="1"/>
+      <c r="AN26" s="11"/>
+      <c r="AO26" s="1"/>
+      <c r="AP26" s="1"/>
+      <c r="AQ26" s="1"/>
+      <c r="AR26" s="1"/>
+      <c r="AS26" s="1"/>
+      <c r="AT26" s="1"/>
+      <c r="AU26" s="1"/>
+      <c r="AV26" s="1"/>
+      <c r="AW26" s="1"/>
+      <c r="AX26" s="13"/>
+      <c r="AY26" s="1"/>
+      <c r="AZ26" s="1"/>
+      <c r="BA26" s="1"/>
+      <c r="BB26" s="2"/>
+      <c r="BC26" s="3"/>
+      <c r="BD26" s="3"/>
+      <c r="BE26" s="3"/>
+      <c r="BF26" s="3"/>
+      <c r="BG26" s="3"/>
+      <c r="BH26" s="3"/>
+      <c r="BI26" s="3"/>
+      <c r="BJ26" s="3"/>
+      <c r="BK26" s="3"/>
+      <c r="BL26" s="3"/>
+    </row>
+    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="1"/>
+      <c r="AF27" s="1"/>
+      <c r="AG27" s="1"/>
+      <c r="AH27" s="1"/>
+      <c r="AI27" s="1"/>
+      <c r="AJ27" s="1"/>
+      <c r="AK27" s="1"/>
+      <c r="AL27" s="1"/>
+      <c r="AM27" s="1"/>
+      <c r="AN27" s="11"/>
+      <c r="AO27" s="1"/>
+      <c r="AP27" s="1"/>
+      <c r="AQ27" s="1"/>
+      <c r="AR27" s="1"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1"/>
+      <c r="AU27" s="1"/>
+      <c r="AV27" s="1"/>
+      <c r="AW27" s="1"/>
+      <c r="AY27" s="1"/>
+      <c r="AZ27" s="1"/>
+      <c r="BA27" s="1"/>
+      <c r="BB27" s="2"/>
+      <c r="BC27" s="3"/>
+      <c r="BD27" s="3"/>
+      <c r="BE27" s="3"/>
+      <c r="BF27" s="3"/>
+      <c r="BG27" s="3"/>
+      <c r="BH27" s="3"/>
+      <c r="BI27" s="3"/>
+      <c r="BJ27" s="3"/>
+      <c r="BK27" s="3"/>
+      <c r="BL27" s="3"/>
+    </row>
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="1"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="1"/>
+      <c r="AF28" s="1"/>
+      <c r="AG28" s="1"/>
+      <c r="AH28" s="1"/>
+      <c r="AI28" s="1"/>
+      <c r="AJ28" s="1"/>
+      <c r="AK28" s="1"/>
+      <c r="AL28" s="1"/>
+      <c r="AM28" s="1"/>
+      <c r="AN28" s="11"/>
+      <c r="AO28" s="1"/>
+      <c r="AP28" s="1"/>
+      <c r="AQ28" s="1"/>
+      <c r="AR28" s="1"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1"/>
+      <c r="AU28" s="1"/>
+      <c r="AV28" s="1"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="13"/>
+      <c r="AY28" s="1"/>
+      <c r="AZ28" s="1"/>
+      <c r="BA28" s="1"/>
+      <c r="BB28" s="2"/>
+      <c r="BC28" s="3"/>
+      <c r="BD28" s="3"/>
+      <c r="BE28" s="3"/>
+      <c r="BF28" s="3"/>
+      <c r="BG28" s="3"/>
+      <c r="BH28" s="3"/>
+      <c r="BI28" s="3"/>
+      <c r="BJ28" s="3"/>
+      <c r="BK28" s="3"/>
+      <c r="BL28" s="3"/>
+    </row>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="1"/>
+      <c r="AF29" s="1"/>
+      <c r="AG29" s="1"/>
+      <c r="AH29" s="1"/>
+      <c r="AI29" s="1"/>
+      <c r="AJ29" s="1"/>
+      <c r="AK29" s="1"/>
+      <c r="AL29" s="1"/>
+      <c r="AM29" s="1"/>
+      <c r="AN29" s="11"/>
+      <c r="AO29" s="1"/>
+      <c r="AP29" s="1"/>
+      <c r="AQ29" s="1"/>
+      <c r="AR29" s="1"/>
+      <c r="AS29" s="1"/>
+      <c r="AT29" s="1"/>
+      <c r="AU29" s="1"/>
+      <c r="AV29" s="1"/>
+      <c r="AW29" s="1"/>
+      <c r="AX29" s="13"/>
+      <c r="AY29" s="1"/>
+      <c r="AZ29" s="1"/>
+      <c r="BA29" s="1"/>
+      <c r="BB29" s="2"/>
+      <c r="BC29" s="3"/>
+      <c r="BD29" s="3"/>
+      <c r="BE29" s="3"/>
+      <c r="BF29" s="3"/>
+      <c r="BG29" s="3"/>
+      <c r="BH29" s="3"/>
+      <c r="BI29" s="3"/>
+      <c r="BJ29" s="3"/>
+      <c r="BK29" s="3"/>
+      <c r="BL29" s="3"/>
+    </row>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="15"/>
+      <c r="O30" s="15"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
+      <c r="S30" s="15"/>
+      <c r="T30" s="17"/>
+      <c r="U30" s="15"/>
+      <c r="V30" s="15"/>
+      <c r="W30" s="15"/>
+      <c r="X30" s="15"/>
+      <c r="Y30" s="15"/>
+      <c r="Z30" s="15"/>
+      <c r="AA30" s="15"/>
+      <c r="AB30" s="15"/>
+      <c r="AC30" s="15"/>
+      <c r="AD30" s="18"/>
+      <c r="AE30" s="15"/>
+      <c r="AF30" s="15"/>
+      <c r="AG30" s="15"/>
+      <c r="AH30" s="15"/>
+      <c r="AI30" s="15"/>
+      <c r="AJ30" s="15"/>
+      <c r="AK30" s="15"/>
+      <c r="AL30" s="15"/>
+      <c r="AM30" s="15"/>
+      <c r="AN30" s="22"/>
+      <c r="AO30" s="15"/>
+      <c r="AP30" s="15"/>
+      <c r="AQ30" s="15"/>
+      <c r="AR30" s="15"/>
+      <c r="AS30" s="15"/>
+      <c r="AT30" s="15"/>
+      <c r="AU30" s="15"/>
+      <c r="AV30" s="15"/>
+      <c r="AW30" s="15"/>
+      <c r="AX30" s="23"/>
+      <c r="AY30" s="15"/>
+      <c r="AZ30" s="15"/>
+      <c r="BA30" s="15"/>
+      <c r="BB30" s="24"/>
+      <c r="BC30" s="3"/>
+      <c r="BD30" s="3"/>
+      <c r="BE30" s="3"/>
+      <c r="BF30" s="3"/>
+      <c r="BG30" s="3"/>
+      <c r="BH30" s="3"/>
+      <c r="BI30" s="3"/>
+      <c r="BJ30" s="3"/>
+      <c r="BK30" s="3"/>
+      <c r="BL30" s="3"/>
+    </row>
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="20"/>
+      <c r="U31" s="3"/>
+      <c r="V31" s="3"/>
+      <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
+      <c r="Y31" s="3"/>
+      <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
+      <c r="AB31" s="3"/>
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="21"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
+      <c r="AG31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
+      <c r="AN31" s="25"/>
+      <c r="AO31" s="3"/>
+      <c r="AP31" s="3"/>
+      <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
+      <c r="AS31" s="3"/>
+      <c r="AT31" s="3"/>
+      <c r="AU31" s="3"/>
+      <c r="AV31" s="3"/>
+      <c r="AW31" s="3"/>
+      <c r="AX31" s="26"/>
+      <c r="AY31" s="3"/>
+      <c r="AZ31" s="3"/>
+      <c r="BA31" s="3"/>
+      <c r="BB31" s="3"/>
+      <c r="BC31" s="3"/>
+      <c r="BD31" s="3"/>
+      <c r="BE31" s="3"/>
+      <c r="BF31" s="3"/>
+      <c r="BG31" s="3"/>
+      <c r="BH31" s="3"/>
+      <c r="BI31" s="3"/>
+      <c r="BJ31" s="3"/>
+      <c r="BK31" s="3"/>
+      <c r="BL31" s="3"/>
+    </row>
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="20"/>
+      <c r="U32" s="3"/>
+      <c r="V32" s="3"/>
+      <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3"/>
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="21"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
+      <c r="AM32" s="3"/>
+      <c r="AN32" s="25"/>
+      <c r="AO32" s="3"/>
+      <c r="AP32" s="3"/>
+      <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
+      <c r="AS32" s="3"/>
+      <c r="AT32" s="3"/>
+      <c r="AU32" s="3"/>
+      <c r="AV32" s="3"/>
+      <c r="AW32" s="3"/>
+      <c r="AX32" s="26"/>
+      <c r="AY32" s="3"/>
+      <c r="AZ32" s="3"/>
+      <c r="BA32" s="3"/>
+      <c r="BB32" s="3"/>
+      <c r="BC32" s="3"/>
+      <c r="BD32" s="3"/>
+      <c r="BE32" s="3"/>
+      <c r="BF32" s="3"/>
+      <c r="BG32" s="3"/>
+      <c r="BH32" s="3"/>
+      <c r="BI32" s="3"/>
+      <c r="BJ32" s="3"/>
+      <c r="BK32" s="3"/>
+      <c r="BL32" s="3"/>
+    </row>
+    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="20"/>
+      <c r="U33" s="3"/>
+      <c r="V33" s="3"/>
+      <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
+      <c r="Y33" s="3"/>
+      <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
+      <c r="AB33" s="3"/>
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="21"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
+      <c r="AG33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="3"/>
+      <c r="AM33" s="3"/>
+      <c r="AN33" s="25"/>
+      <c r="AO33" s="3"/>
+      <c r="AP33" s="3"/>
+      <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
+      <c r="AS33" s="3"/>
+      <c r="AT33" s="3"/>
+      <c r="AU33" s="3"/>
+      <c r="AV33" s="3"/>
+      <c r="AW33" s="3"/>
+      <c r="AX33" s="26"/>
+      <c r="AY33" s="3"/>
+      <c r="AZ33" s="3"/>
+      <c r="BA33" s="3"/>
+      <c r="BB33" s="3"/>
+      <c r="BC33" s="3"/>
+      <c r="BD33" s="3"/>
+      <c r="BE33" s="3"/>
+      <c r="BF33" s="3"/>
+      <c r="BG33" s="3"/>
+      <c r="BH33" s="3"/>
+      <c r="BI33" s="3"/>
+      <c r="BJ33" s="3"/>
+      <c r="BK33" s="3"/>
+      <c r="BL33" s="3"/>
+    </row>
+    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="20"/>
+      <c r="U34" s="3"/>
+      <c r="V34" s="3"/>
+      <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3"/>
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="21"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3"/>
+      <c r="AL34" s="3"/>
+      <c r="AM34" s="3"/>
+      <c r="AN34" s="25"/>
+      <c r="AO34" s="3"/>
+      <c r="AP34" s="3"/>
+      <c r="AQ34" s="3"/>
+      <c r="AR34" s="3"/>
+      <c r="AS34" s="3"/>
+      <c r="AT34" s="3"/>
+      <c r="AU34" s="3"/>
+      <c r="AV34" s="3"/>
+      <c r="AW34" s="3"/>
+      <c r="AX34" s="26"/>
+      <c r="AY34" s="3"/>
+      <c r="AZ34" s="3"/>
+      <c r="BA34" s="3"/>
+      <c r="BB34" s="3"/>
+      <c r="BC34" s="3"/>
+      <c r="BD34" s="3"/>
+      <c r="BE34" s="3"/>
+      <c r="BF34" s="3"/>
+      <c r="BG34" s="3"/>
+      <c r="BH34" s="3"/>
+      <c r="BI34" s="3"/>
+      <c r="BJ34" s="3"/>
+      <c r="BK34" s="3"/>
+      <c r="BL34" s="3"/>
+    </row>
+    <row r="36" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AT36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="AU39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
start bg changed home basse added respozive added but not working
</commit_message>
<xml_diff>
--- a/GUI_20212202_AYZ8R9/Maps/map.xlsx
+++ b/GUI_20212202_AYZ8R9/Maps/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\game3\GUI_20212202_AYZ8R9\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409971BD-C55B-411D-8B15-D553E955361D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CEDD5E-9C07-41CB-ABFE-CB069851AD42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="4" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="17">
   <si>
     <t>B</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>HOME</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -525,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382D7427-FBDE-4BF3-ADAB-21A4C37623DD}">
   <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
@@ -2799,8 +2802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32EA023-0038-482A-B633-0391C0CB8525}">
   <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3380,7 +3383,7 @@
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AJ9" s="1" t="s">
         <v>1</v>
@@ -3450,10 +3453,10 @@
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AJ10" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AK10" s="1" t="s">
         <v>1</v>
@@ -3476,15 +3479,9 @@
       <c r="AY10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AZ10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BA10" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="BB10" s="2" t="s">
-        <v>0</v>
-      </c>
+      <c r="AZ10" s="1"/>
+      <c r="BA10" s="1"/>
+      <c r="BB10" s="2"/>
       <c r="BC10" s="3"/>
       <c r="BD10" s="3"/>
       <c r="BE10" s="3"/>
@@ -3532,13 +3529,13 @@
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AJ11" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AK11" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AL11" s="1" t="s">
         <v>1</v>
@@ -3557,19 +3554,19 @@
         <v>4</v>
       </c>
       <c r="AX11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA11" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AY11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA11" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="BB11" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="BC11" s="3"/>
       <c r="BD11" s="3"/>
@@ -3618,16 +3615,16 @@
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AJ12" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AK12" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AL12" s="27" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AM12" s="1" t="s">
         <v>1</v>
@@ -3644,22 +3641,22 @@
         <v>4</v>
       </c>
       <c r="AW12" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AX12" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA12" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AY12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA12" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="BB12" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="BC12" s="3"/>
       <c r="BD12" s="3"/>
@@ -3726,19 +3723,19 @@
       </c>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AJ13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AK13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AL13" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="AM13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AN13" s="11" t="s">
         <v>1</v>
@@ -3753,25 +3750,25 @@
         <v>4</v>
       </c>
       <c r="AV13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AW13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AX13" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AY13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA13" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="BB13" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="BC13" s="3"/>
       <c r="BD13" s="3"/>
@@ -3828,22 +3825,22 @@
         <v>5</v>
       </c>
       <c r="AI14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ14" s="27" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AJ14" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="AK14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AL14" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="AM14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AN14" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AO14" s="1" t="s">
         <v>1</v>
@@ -3864,28 +3861,28 @@
         <v>0</v>
       </c>
       <c r="AU14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AV14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AW14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AX14" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AY14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA14" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="BB14" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="BC14" s="3"/>
       <c r="BD14" s="3"/>
@@ -3943,58 +3940,58 @@
         <v>5</v>
       </c>
       <c r="AJ15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AK15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AL15" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="AM15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AN15" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AO15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AP15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AQ15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AR15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AS15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AT15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AU15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AV15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AW15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AX15" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="AY15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AZ15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="BA15" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AY15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="AZ15" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="BA15" s="13" t="s">
+        <v>16</v>
       </c>
       <c r="BB15" s="1" t="s">
         <v>12</v>
@@ -4066,43 +4063,43 @@
         <v>5</v>
       </c>
       <c r="AK16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AL16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
+      </c>
+      <c r="AL16" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="AM16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AN16" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AO16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AP16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AQ16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AR16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AS16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AT16" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AU16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AV16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AW16" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AX16" s="13"/>
       <c r="AY16" s="1" t="s">
@@ -4182,41 +4179,41 @@
       <c r="AK17" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="AL17" s="1" t="s">
-        <v>9</v>
+      <c r="AL17" s="27" t="s">
+        <v>16</v>
       </c>
       <c r="AM17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AN17" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AO17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AP17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AQ17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AR17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AS17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AT17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AU17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AV17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AW17" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AX17" s="13" t="s">
         <v>5</v>
@@ -4302,34 +4299,34 @@
         <v>5</v>
       </c>
       <c r="AM18" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AN18" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AO18" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AP18" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AQ18" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AR18" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AS18" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AT18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AU18" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AV18" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AW18" s="1" t="s">
         <v>5</v>
@@ -4409,28 +4406,28 @@
         <v>5</v>
       </c>
       <c r="AN19" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AO19" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AP19" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AQ19" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AR19" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AS19" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AT19" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AU19" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="AV19" t="s">
         <v>5</v>
@@ -5523,8 +5520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8F6284-F138-4CEB-A50F-8C3CA6F27EB7}">
   <dimension ref="A1:BL34"/>
   <sheetViews>
-    <sheetView topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AX13" sqref="AX13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8170,7 +8167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="AD1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
npc fight select wondow added
</commit_message>
<xml_diff>
--- a/GUI_20212202_AYZ8R9/Maps/map.xlsx
+++ b/GUI_20212202_AYZ8R9/Maps/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\game5\GUI_20212202_AYZ8R9\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0933D29-9A61-48F8-9CFE-96E55A86DF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B7339E-0304-4C64-AD84-6982B66B015B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4890" yWindow="615" windowWidth="21600" windowHeight="13575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="29">
   <si>
     <t>B</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>HOMERW</t>
-  </si>
-  <si>
-    <t>P1</t>
   </si>
   <si>
     <t>P2</t>
@@ -708,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382D7427-FBDE-4BF3-ADAB-21A4C37623DD}">
   <dimension ref="A1:CY47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" topLeftCell="S7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AL15" sqref="AL15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2753,25 +2750,25 @@
         <v>23</v>
       </c>
       <c r="Z19" s="44" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="AA19" s="44" t="s">
         <v>23</v>
       </c>
       <c r="AB19" s="44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC19" s="44" t="s">
         <v>23</v>
       </c>
       <c r="AD19" s="44" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="AE19" s="44" t="s">
         <v>23</v>
       </c>
       <c r="AF19" s="44" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="AG19" s="44" t="s">
         <v>19</v>
@@ -2791,7 +2788,7 @@
       <c r="AR19" s="44"/>
       <c r="AS19" s="44"/>
       <c r="AT19" s="44"/>
-      <c r="AU19" s="44"/>
+      <c r="AU19" s="1"/>
       <c r="AV19" s="44"/>
       <c r="AW19" s="44"/>
       <c r="AX19" s="49"/>
@@ -5839,7 +5836,7 @@
   <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="U17" sqref="U17"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6837,10 +6834,14 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="I16" s="1"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="1"/>
+      <c r="K16" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -8299,7 +8300,7 @@
   <dimension ref="A1:BL35"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10893,7 +10894,7 @@
   <dimension ref="A1:BL40"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13360,8 +13361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9BF40A-B043-489B-97BD-E120A8256F34}">
   <dimension ref="A1:CY47"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AK28" sqref="AK28"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16008,6 +16009,9 @@
         <v>8</v>
       </c>
       <c r="Z24" s="44"/>
+      <c r="AA24" s="44" t="s">
+        <v>17</v>
+      </c>
       <c r="AB24" s="44"/>
       <c r="AD24" s="47"/>
       <c r="AE24" s="44"/>
@@ -16488,9 +16492,6 @@
       <c r="AH28" s="44"/>
       <c r="AI28" s="44"/>
       <c r="AJ28" s="44"/>
-      <c r="AK28" s="44" t="s">
-        <v>17</v>
-      </c>
       <c r="AM28" s="44"/>
       <c r="AN28" s="44"/>
       <c r="AO28" s="44"/>
@@ -20718,7 +20719,7 @@
   <dimension ref="A1:BC32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AJ26" sqref="AJ26"/>
+      <selection activeCell="AQ22" sqref="AQ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22095,7 +22096,9 @@
       <c r="AN22" s="48"/>
       <c r="AO22" s="44"/>
       <c r="AP22" s="44"/>
-      <c r="AR22" s="44"/>
+      <c r="AQ22" s="44" t="s">
+        <v>17</v>
+      </c>
       <c r="AS22" s="44" t="s">
         <v>8</v>
       </c>
@@ -22351,9 +22354,6 @@
       <c r="AG26" s="44"/>
       <c r="AH26" s="44"/>
       <c r="AI26" s="44"/>
-      <c r="AJ26" s="44" t="s">
-        <v>17</v>
-      </c>
       <c r="AK26" s="44"/>
       <c r="AL26" s="44" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
map chest db fix
</commit_message>
<xml_diff>
--- a/GUI_20212202_AYZ8R9/Maps/map.xlsx
+++ b/GUI_20212202_AYZ8R9/Maps/map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krisz\OneDrive\Asztali gép\SZTGUI Féléves\GUI_20212202_AYZ8R9\GUI_20212202_AYZ8R9\Maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\game6\GUI_20212202_AYZ8R9\Maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{447FFAEC-4886-4786-A2B8-8D14EC9C0806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E621FE3-E569-48F3-8092-8B7CDE800310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="29">
   <si>
     <t>B</t>
   </si>
@@ -706,27 +706,27 @@
   <dimension ref="A1:CY47"/>
   <sheetViews>
     <sheetView topLeftCell="S7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="AL15" sqref="AL15"/>
+      <selection activeCell="AG19" sqref="AG19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="4.33203125" style="29"/>
-    <col min="10" max="10" width="4.33203125" style="36"/>
-    <col min="11" max="19" width="4.33203125" style="29"/>
-    <col min="20" max="20" width="4.33203125" style="37"/>
-    <col min="21" max="29" width="4.33203125" style="29"/>
-    <col min="30" max="30" width="4.33203125" style="38"/>
-    <col min="31" max="39" width="4.33203125" style="29"/>
-    <col min="40" max="40" width="4.33203125" style="39"/>
-    <col min="41" max="49" width="4.33203125" style="29"/>
-    <col min="50" max="50" width="4.33203125" style="40"/>
-    <col min="51" max="54" width="4.33203125" style="29"/>
-    <col min="55" max="55" width="4.33203125" style="43"/>
-    <col min="56" max="16384" width="4.33203125" style="29"/>
+    <col min="1" max="9" width="4.28515625" style="29"/>
+    <col min="10" max="10" width="4.28515625" style="36"/>
+    <col min="11" max="19" width="4.28515625" style="29"/>
+    <col min="20" max="20" width="4.28515625" style="37"/>
+    <col min="21" max="29" width="4.28515625" style="29"/>
+    <col min="30" max="30" width="4.28515625" style="38"/>
+    <col min="31" max="39" width="4.28515625" style="29"/>
+    <col min="40" max="40" width="4.28515625" style="39"/>
+    <col min="41" max="49" width="4.28515625" style="29"/>
+    <col min="50" max="50" width="4.28515625" style="40"/>
+    <col min="51" max="54" width="4.28515625" style="29"/>
+    <col min="55" max="55" width="4.28515625" style="43"/>
+    <col min="56" max="16384" width="4.28515625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:103" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="62"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -830,7 +830,7 @@
       <c r="CX1" s="64"/>
       <c r="CY1" s="64"/>
     </row>
-    <row r="2" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -937,7 +937,7 @@
       <c r="CX2" s="28"/>
       <c r="CY2" s="28"/>
     </row>
-    <row r="3" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -1044,7 +1044,7 @@
       <c r="CX3" s="28"/>
       <c r="CY3" s="28"/>
     </row>
-    <row r="4" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -1151,7 +1151,7 @@
       <c r="CX4" s="28"/>
       <c r="CY4" s="28"/>
     </row>
-    <row r="5" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -1258,7 +1258,7 @@
       <c r="CX5" s="28"/>
       <c r="CY5" s="28"/>
     </row>
-    <row r="6" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -1365,7 +1365,7 @@
       <c r="CX6" s="28"/>
       <c r="CY6" s="28"/>
     </row>
-    <row r="7" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
@@ -1472,7 +1472,7 @@
       <c r="CX7" s="28"/>
       <c r="CY7" s="28"/>
     </row>
-    <row r="8" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -1579,7 +1579,7 @@
       <c r="CX8" s="28"/>
       <c r="CY8" s="28"/>
     </row>
-    <row r="9" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -1686,7 +1686,7 @@
       <c r="CX9" s="28"/>
       <c r="CY9" s="28"/>
     </row>
-    <row r="10" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -1793,7 +1793,7 @@
       <c r="CX10" s="28"/>
       <c r="CY10" s="28"/>
     </row>
-    <row r="11" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -1900,7 +1900,7 @@
       <c r="CX11" s="28"/>
       <c r="CY11" s="28"/>
     </row>
-    <row r="12" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
@@ -2007,7 +2007,7 @@
       <c r="CX12" s="28"/>
       <c r="CY12" s="28"/>
     </row>
-    <row r="13" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -2114,7 +2114,7 @@
       <c r="CX13" s="28"/>
       <c r="CY13" s="28"/>
     </row>
-    <row r="14" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
@@ -2221,7 +2221,7 @@
       <c r="CX14" s="28"/>
       <c r="CY14" s="28"/>
     </row>
-    <row r="15" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
@@ -2328,7 +2328,7 @@
       <c r="CX15" s="28"/>
       <c r="CY15" s="28"/>
     </row>
-    <row r="16" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
@@ -2457,7 +2457,7 @@
       <c r="CX16" s="28"/>
       <c r="CY16" s="28"/>
     </row>
-    <row r="17" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -2586,7 +2586,7 @@
       <c r="CX17" s="28"/>
       <c r="CY17" s="28"/>
     </row>
-    <row r="18" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -2715,7 +2715,7 @@
       <c r="CX18" s="28"/>
       <c r="CY18" s="28"/>
     </row>
-    <row r="19" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -2850,7 +2850,7 @@
       <c r="CX19" s="28"/>
       <c r="CY19" s="28"/>
     </row>
-    <row r="20" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
         <v>0</v>
       </c>
@@ -3065,7 +3065,7 @@
       <c r="CX20" s="28"/>
       <c r="CY20" s="28"/>
     </row>
-    <row r="21" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -3172,7 +3172,7 @@
       <c r="CX21" s="28"/>
       <c r="CY21" s="28"/>
     </row>
-    <row r="22" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -3279,7 +3279,7 @@
       <c r="CX22" s="28"/>
       <c r="CY22" s="28"/>
     </row>
-    <row r="23" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -3386,7 +3386,7 @@
       <c r="CX23" s="28"/>
       <c r="CY23" s="28"/>
     </row>
-    <row r="24" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -3493,7 +3493,7 @@
       <c r="CX24" s="28"/>
       <c r="CY24" s="28"/>
     </row>
-    <row r="25" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -3600,7 +3600,7 @@
       <c r="CX25" s="28"/>
       <c r="CY25" s="28"/>
     </row>
-    <row r="26" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -3707,7 +3707,7 @@
       <c r="CX26" s="28"/>
       <c r="CY26" s="28"/>
     </row>
-    <row r="27" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -3814,7 +3814,7 @@
       <c r="CX27" s="28"/>
       <c r="CY27" s="28"/>
     </row>
-    <row r="28" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -3921,7 +3921,7 @@
       <c r="CX28" s="28"/>
       <c r="CY28" s="28"/>
     </row>
-    <row r="29" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -4028,7 +4028,7 @@
       <c r="CX29" s="28"/>
       <c r="CY29" s="28"/>
     </row>
-    <row r="30" spans="1:103" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:103" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="54"/>
       <c r="B30" s="54"/>
       <c r="C30" s="54"/>
@@ -4135,7 +4135,7 @@
       <c r="CX30" s="28"/>
       <c r="CY30" s="28"/>
     </row>
-    <row r="31" spans="1:103" s="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:103" s="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC31" s="51">
         <v>29</v>
       </c>
@@ -4188,7 +4188,7 @@
       <c r="CX31" s="67"/>
       <c r="CY31" s="67"/>
     </row>
-    <row r="32" spans="1:103" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:103" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="53">
         <v>0</v>
       </c>
@@ -4401,7 +4401,7 @@
       <c r="CX32" s="28"/>
       <c r="CY32" s="28"/>
     </row>
-    <row r="33" spans="1:103" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:103" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -4506,7 +4506,7 @@
       <c r="CX33" s="28"/>
       <c r="CY33" s="28"/>
     </row>
-    <row r="34" spans="1:103" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:103" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J34" s="30"/>
       <c r="T34" s="31"/>
       <c r="AD34" s="32"/>
@@ -4514,7 +4514,7 @@
       <c r="AX34" s="34"/>
       <c r="BC34" s="35"/>
     </row>
-    <row r="35" spans="1:103" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:103" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
@@ -4619,7 +4619,7 @@
       <c r="CX35" s="28"/>
       <c r="CY35" s="28"/>
     </row>
-    <row r="36" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28"/>
       <c r="B36" s="28"/>
       <c r="C36" s="28"/>
@@ -4724,7 +4724,7 @@
       <c r="CX36" s="28"/>
       <c r="CY36" s="28"/>
     </row>
-    <row r="37" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
@@ -4829,7 +4829,7 @@
       <c r="CX37" s="28"/>
       <c r="CY37" s="28"/>
     </row>
-    <row r="38" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
@@ -4934,7 +4934,7 @@
       <c r="CX38" s="28"/>
       <c r="CY38" s="28"/>
     </row>
-    <row r="39" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
@@ -5039,7 +5039,7 @@
       <c r="CX39" s="28"/>
       <c r="CY39" s="28"/>
     </row>
-    <row r="40" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
       <c r="B40" s="28"/>
       <c r="C40" s="28"/>
@@ -5144,7 +5144,7 @@
       <c r="CX40" s="28"/>
       <c r="CY40" s="28"/>
     </row>
-    <row r="41" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28"/>
       <c r="B41" s="28"/>
       <c r="C41" s="28"/>
@@ -5249,7 +5249,7 @@
       <c r="CX41" s="28"/>
       <c r="CY41" s="28"/>
     </row>
-    <row r="42" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28"/>
       <c r="B42" s="28"/>
       <c r="C42" s="28"/>
@@ -5354,7 +5354,7 @@
       <c r="CX42" s="28"/>
       <c r="CY42" s="28"/>
     </row>
-    <row r="43" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
       <c r="B43" s="28"/>
       <c r="C43" s="28"/>
@@ -5459,7 +5459,7 @@
       <c r="CX43" s="28"/>
       <c r="CY43" s="28"/>
     </row>
-    <row r="44" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
       <c r="B44" s="28"/>
       <c r="C44" s="28"/>
@@ -5564,7 +5564,7 @@
       <c r="CX44" s="28"/>
       <c r="CY44" s="28"/>
     </row>
-    <row r="45" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
       <c r="B45" s="28"/>
       <c r="C45" s="28"/>
@@ -5669,7 +5669,7 @@
       <c r="CX45" s="28"/>
       <c r="CY45" s="28"/>
     </row>
-    <row r="46" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
       <c r="B46" s="28"/>
       <c r="C46" s="28"/>
@@ -5774,7 +5774,7 @@
       <c r="CX46" s="28"/>
       <c r="CY46" s="28"/>
     </row>
-    <row r="47" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC47" s="41"/>
       <c r="BD47" s="42"/>
       <c r="BE47" s="42"/>
@@ -5835,21 +5835,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B32EA023-0038-482A-B633-0391C0CB8525}">
   <dimension ref="A1:BL35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AH25" sqref="AH25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="4.44140625" style="6"/>
-    <col min="20" max="20" width="4.44140625" style="8"/>
-    <col min="30" max="30" width="4.44140625" style="10"/>
-    <col min="40" max="40" width="4.44140625" style="12"/>
-    <col min="50" max="50" width="4.44140625" style="14"/>
+    <col min="10" max="10" width="4.42578125" style="6"/>
+    <col min="20" max="20" width="4.42578125" style="8"/>
+    <col min="30" max="30" width="4.42578125" style="10"/>
+    <col min="40" max="40" width="4.42578125" style="12"/>
+    <col min="50" max="50" width="4.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="68" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" s="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -5915,7 +5915,7 @@
       <c r="BK2" s="3"/>
       <c r="BL2" s="3"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -5981,7 +5981,7 @@
       <c r="BK3" s="3"/>
       <c r="BL3" s="3"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -6047,7 +6047,7 @@
       <c r="BK4" s="3"/>
       <c r="BL4" s="3"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -6113,7 +6113,7 @@
       <c r="BK5" s="3"/>
       <c r="BL5" s="3"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -6179,7 +6179,7 @@
       <c r="BK6" s="3"/>
       <c r="BL6" s="3"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -6245,7 +6245,7 @@
       <c r="BK7" s="3"/>
       <c r="BL7" s="3"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -6311,7 +6311,7 @@
       <c r="BK8" s="3"/>
       <c r="BL8" s="3"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -6381,7 +6381,7 @@
       <c r="BK9" s="3"/>
       <c r="BL9" s="3"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -6451,7 +6451,7 @@
       <c r="BK10" s="3"/>
       <c r="BL10" s="3"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -6520,7 +6520,7 @@
       <c r="BK11" s="3"/>
       <c r="BL11" s="3"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -6590,7 +6590,7 @@
       <c r="BK12" s="3"/>
       <c r="BL12" s="3"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -6660,7 +6660,7 @@
       <c r="BK13" s="3"/>
       <c r="BL13" s="3"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -6760,7 +6760,7 @@
       <c r="BK14" s="3"/>
       <c r="BL14" s="3"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -6826,7 +6826,7 @@
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -6834,9 +6834,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="5"/>
       <c r="K16" s="1"/>
@@ -6902,7 +6900,7 @@
       <c r="BK16" s="3"/>
       <c r="BL16" s="3"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -6994,7 +6992,7 @@
       <c r="BK17" s="3"/>
       <c r="BL17" s="3"/>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -7076,7 +7074,7 @@
       <c r="BK18" s="3"/>
       <c r="BL18" s="3"/>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -7159,7 +7157,7 @@
       <c r="BK19" s="3"/>
       <c r="BL19" s="3"/>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
@@ -7233,7 +7231,7 @@
       <c r="BK20" s="3"/>
       <c r="BL20" s="3"/>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -7329,7 +7327,7 @@
       <c r="BK21" s="3"/>
       <c r="BL21" s="3"/>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -7401,7 +7399,7 @@
       <c r="BK22" s="3"/>
       <c r="BL22" s="3"/>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -7471,7 +7469,7 @@
       <c r="BK23" s="3"/>
       <c r="BL23" s="3"/>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -7541,7 +7539,7 @@
       <c r="BK24" s="3"/>
       <c r="BL24" s="3"/>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -7611,7 +7609,7 @@
       <c r="BK25" s="3"/>
       <c r="BL25" s="3"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -7683,7 +7681,7 @@
       <c r="BK26" s="3"/>
       <c r="BL26" s="3"/>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -7761,7 +7759,7 @@
       <c r="BK27" s="3"/>
       <c r="BL27" s="3"/>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -7826,7 +7824,7 @@
       <c r="BK28" s="3"/>
       <c r="BL28" s="3"/>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -7892,7 +7890,7 @@
       <c r="BK29" s="3"/>
       <c r="BL29" s="3"/>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -7958,7 +7956,7 @@
       <c r="BK30" s="3"/>
       <c r="BL30" s="3"/>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -8024,7 +8022,7 @@
       <c r="BK31" s="3"/>
       <c r="BL31" s="3"/>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -8090,7 +8088,7 @@
       <c r="BK32" s="3"/>
       <c r="BL32" s="3"/>
     </row>
-    <row r="33" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -8156,7 +8154,7 @@
       <c r="BK33" s="3"/>
       <c r="BL33" s="3"/>
     </row>
-    <row r="34" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -8222,7 +8220,7 @@
       <c r="BK34" s="3"/>
       <c r="BL34" s="3"/>
     </row>
-    <row r="35" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -8297,21 +8295,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8F6284-F138-4CEB-A50F-8C3CA6F27EB7}">
   <dimension ref="A1:BL35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="4.44140625" style="6"/>
-    <col min="20" max="20" width="4.44140625" style="8"/>
-    <col min="30" max="30" width="4.44140625" style="10"/>
-    <col min="40" max="40" width="4.44140625" style="12"/>
-    <col min="50" max="50" width="4.44140625" style="14"/>
+    <col min="10" max="10" width="4.42578125" style="6"/>
+    <col min="20" max="20" width="4.42578125" style="8"/>
+    <col min="30" max="30" width="4.42578125" style="10"/>
+    <col min="40" max="40" width="4.42578125" style="12"/>
+    <col min="50" max="50" width="4.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="68" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" s="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -8377,7 +8375,7 @@
       <c r="BK2" s="3"/>
       <c r="BL2" s="3"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -8443,7 +8441,7 @@
       <c r="BK3" s="3"/>
       <c r="BL3" s="3"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -8509,7 +8507,7 @@
       <c r="BK4" s="3"/>
       <c r="BL4" s="3"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -8577,7 +8575,7 @@
       <c r="BK5" s="3"/>
       <c r="BL5" s="3"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -8652,7 +8650,7 @@
       <c r="BK6" s="3"/>
       <c r="BL6" s="3"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -8748,7 +8746,7 @@
       <c r="BK7" s="3"/>
       <c r="BL7" s="3"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -8830,7 +8828,7 @@
       <c r="BK8" s="3"/>
       <c r="BL8" s="3"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
@@ -8912,7 +8910,7 @@
       <c r="BK9" s="3"/>
       <c r="BL9" s="3"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -8996,7 +8994,7 @@
       <c r="BK10" s="3"/>
       <c r="BL10" s="3"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="5"/>
@@ -9067,7 +9065,7 @@
       <c r="BK11" s="3"/>
       <c r="BL11" s="3"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -9075,9 +9073,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="5"/>
       <c r="K12" s="1"/>
@@ -9147,7 +9143,7 @@
       <c r="BK12" s="3"/>
       <c r="BL12" s="3"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -9243,7 +9239,7 @@
       <c r="BK13" s="3"/>
       <c r="BL13" s="3"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -9329,7 +9325,7 @@
       <c r="BK14" s="3"/>
       <c r="BL14" s="3"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -9409,7 +9405,7 @@
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -9493,7 +9489,7 @@
       <c r="BK16" s="3"/>
       <c r="BL16" s="3"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -9581,7 +9577,7 @@
       <c r="BK17" s="3"/>
       <c r="BL17" s="3"/>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -9665,7 +9661,7 @@
       <c r="BK18" s="3"/>
       <c r="BL18" s="3"/>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -9745,7 +9741,7 @@
       <c r="BK19" s="3"/>
       <c r="BL19" s="3"/>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -9828,7 +9824,7 @@
       <c r="BK20" s="3"/>
       <c r="BL20" s="3"/>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -9896,7 +9892,7 @@
       <c r="BK21" s="3"/>
       <c r="BL21" s="3"/>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -9970,7 +9966,7 @@
       <c r="BK22" s="3"/>
       <c r="BL22" s="3"/>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -10044,7 +10040,7 @@
       <c r="BK23" s="3"/>
       <c r="BL23" s="3"/>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -10120,7 +10116,7 @@
       <c r="BK24" s="3"/>
       <c r="BL24" s="3"/>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -10192,7 +10188,7 @@
       <c r="BK25" s="3"/>
       <c r="BL25" s="3"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -10265,7 +10261,7 @@
       <c r="BK26" s="3"/>
       <c r="BL26" s="3"/>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -10353,7 +10349,7 @@
       <c r="BK27" s="3"/>
       <c r="BL27" s="3"/>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -10418,7 +10414,7 @@
       <c r="BK28" s="3"/>
       <c r="BL28" s="3"/>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -10484,7 +10480,7 @@
       <c r="BK29" s="3"/>
       <c r="BL29" s="3"/>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -10550,7 +10546,7 @@
       <c r="BK30" s="3"/>
       <c r="BL30" s="3"/>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -10616,7 +10612,7 @@
       <c r="BK31" s="3"/>
       <c r="BL31" s="3"/>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -10682,7 +10678,7 @@
       <c r="BK32" s="3"/>
       <c r="BL32" s="3"/>
     </row>
-    <row r="33" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -10748,7 +10744,7 @@
       <c r="BK33" s="3"/>
       <c r="BL33" s="3"/>
     </row>
-    <row r="34" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -10814,7 +10810,7 @@
       <c r="BK34" s="3"/>
       <c r="BL34" s="3"/>
     </row>
-    <row r="35" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -10889,21 +10885,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BL40"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="10" max="10" width="4.44140625" style="6"/>
-    <col min="20" max="20" width="4.44140625" style="8"/>
-    <col min="30" max="30" width="4.44140625" style="10"/>
-    <col min="40" max="40" width="4.44140625" style="12"/>
-    <col min="50" max="50" width="4.44140625" style="14"/>
+    <col min="10" max="10" width="4.42578125" style="6"/>
+    <col min="20" max="20" width="4.42578125" style="8"/>
+    <col min="30" max="30" width="4.42578125" style="10"/>
+    <col min="40" max="40" width="4.42578125" style="12"/>
+    <col min="50" max="50" width="4.42578125" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" s="68" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" s="68" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -10969,7 +10965,7 @@
       <c r="BK2" s="3"/>
       <c r="BL2" s="3"/>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -11035,7 +11031,7 @@
       <c r="BK3" s="3"/>
       <c r="BL3" s="3"/>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -11101,7 +11097,7 @@
       <c r="BK4" s="3"/>
       <c r="BL4" s="3"/>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -11167,7 +11163,7 @@
       <c r="BK5" s="3"/>
       <c r="BL5" s="3"/>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -11233,7 +11229,7 @@
       <c r="BK6" s="3"/>
       <c r="BL6" s="3"/>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -11299,7 +11295,7 @@
       <c r="BK7" s="3"/>
       <c r="BL7" s="3"/>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -11365,7 +11361,7 @@
       <c r="BK8" s="3"/>
       <c r="BL8" s="3"/>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -11431,7 +11427,7 @@
       <c r="BK9" s="3"/>
       <c r="BL9" s="3"/>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -11497,7 +11493,7 @@
       <c r="BK10" s="3"/>
       <c r="BL10" s="3"/>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -11563,7 +11559,7 @@
       <c r="BK11" s="3"/>
       <c r="BL11" s="3"/>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -11629,7 +11625,7 @@
       <c r="BK12" s="3"/>
       <c r="BL12" s="3"/>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
@@ -11699,7 +11695,7 @@
       <c r="BK13" s="3"/>
       <c r="BL13" s="3"/>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -11793,7 +11789,7 @@
       <c r="BK14" s="3"/>
       <c r="BL14" s="3"/>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -11871,7 +11867,7 @@
       <c r="BK15" s="3"/>
       <c r="BL15" s="3"/>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>1</v>
@@ -11948,7 +11944,7 @@
       <c r="BK16" s="3"/>
       <c r="BL16" s="3"/>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -12030,7 +12026,7 @@
       <c r="BK17" s="3"/>
       <c r="BL17" s="3"/>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -12108,7 +12104,7 @@
       <c r="BK18" s="3"/>
       <c r="BL18" s="3"/>
     </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -12204,7 +12200,7 @@
       <c r="BK19" s="3"/>
       <c r="BL19" s="3"/>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -12277,7 +12273,7 @@
       <c r="BK20" s="3"/>
       <c r="BL20" s="3"/>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -12369,7 +12365,7 @@
       <c r="BK21" s="3"/>
       <c r="BL21" s="3"/>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -12443,7 +12439,7 @@
       <c r="BK22" s="3"/>
       <c r="BL22" s="3"/>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -12517,7 +12513,7 @@
       <c r="BK23" s="3"/>
       <c r="BL23" s="3"/>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -12591,7 +12587,7 @@
       <c r="BK24" s="3"/>
       <c r="BL24" s="3"/>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -12675,7 +12671,7 @@
       <c r="BK25" s="3"/>
       <c r="BL25" s="3"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -12741,7 +12737,7 @@
       <c r="BK26" s="3"/>
       <c r="BL26" s="3"/>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -12807,7 +12803,7 @@
       <c r="BK27" s="3"/>
       <c r="BL27" s="3"/>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -12872,7 +12868,7 @@
       <c r="BK28" s="3"/>
       <c r="BL28" s="3"/>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -12938,7 +12934,7 @@
       <c r="BK29" s="3"/>
       <c r="BL29" s="3"/>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -13004,7 +13000,7 @@
       <c r="BK30" s="3"/>
       <c r="BL30" s="3"/>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
@@ -13070,7 +13066,7 @@
       <c r="BK31" s="3"/>
       <c r="BL31" s="3"/>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -13136,7 +13132,7 @@
       <c r="BK32" s="3"/>
       <c r="BL32" s="3"/>
     </row>
-    <row r="33" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -13202,7 +13198,7 @@
       <c r="BK33" s="3"/>
       <c r="BL33" s="3"/>
     </row>
-    <row r="34" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -13268,7 +13264,7 @@
       <c r="BK34" s="3"/>
       <c r="BL34" s="3"/>
     </row>
-    <row r="35" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:64" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -13334,12 +13330,12 @@
       <c r="BK35" s="3"/>
       <c r="BL35" s="3"/>
     </row>
-    <row r="37" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:64" x14ac:dyDescent="0.25">
       <c r="AT37" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:64" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:64" x14ac:dyDescent="0.25">
       <c r="AU40" t="s">
         <v>7</v>
       </c>
@@ -13354,28 +13350,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9BF40A-B043-489B-97BD-E120A8256F34}">
   <dimension ref="A1:CY47"/>
   <sheetViews>
-    <sheetView topLeftCell="T4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="AJ25" sqref="AJ25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="4.33203125" style="29"/>
-    <col min="10" max="10" width="4.33203125" style="36"/>
-    <col min="11" max="19" width="4.33203125" style="29"/>
-    <col min="20" max="20" width="4.33203125" style="37"/>
-    <col min="21" max="29" width="4.33203125" style="29"/>
-    <col min="30" max="30" width="4.33203125" style="38"/>
-    <col min="31" max="39" width="4.33203125" style="29"/>
-    <col min="40" max="40" width="4.33203125" style="39"/>
-    <col min="41" max="49" width="4.33203125" style="29"/>
-    <col min="50" max="50" width="4.33203125" style="40"/>
-    <col min="51" max="54" width="4.33203125" style="29"/>
-    <col min="55" max="55" width="4.33203125" style="43"/>
-    <col min="56" max="16384" width="4.33203125" style="29"/>
+    <col min="1" max="9" width="4.28515625" style="29"/>
+    <col min="10" max="10" width="4.28515625" style="36"/>
+    <col min="11" max="19" width="4.28515625" style="29"/>
+    <col min="20" max="20" width="4.28515625" style="37"/>
+    <col min="21" max="29" width="4.28515625" style="29"/>
+    <col min="30" max="30" width="4.28515625" style="38"/>
+    <col min="31" max="39" width="4.28515625" style="29"/>
+    <col min="40" max="40" width="4.28515625" style="39"/>
+    <col min="41" max="49" width="4.28515625" style="29"/>
+    <col min="50" max="50" width="4.28515625" style="40"/>
+    <col min="51" max="54" width="4.28515625" style="29"/>
+    <col min="55" max="55" width="4.28515625" style="43"/>
+    <col min="56" max="16384" width="4.28515625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:103" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="62"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -13479,7 +13475,7 @@
       <c r="CX1" s="64"/>
       <c r="CY1" s="64"/>
     </row>
-    <row r="2" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -13586,7 +13582,7 @@
       <c r="CX2" s="28"/>
       <c r="CY2" s="28"/>
     </row>
-    <row r="3" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -13693,7 +13689,7 @@
       <c r="CX3" s="28"/>
       <c r="CY3" s="28"/>
     </row>
-    <row r="4" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -13800,7 +13796,7 @@
       <c r="CX4" s="28"/>
       <c r="CY4" s="28"/>
     </row>
-    <row r="5" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -13907,7 +13903,7 @@
       <c r="CX5" s="28"/>
       <c r="CY5" s="28"/>
     </row>
-    <row r="6" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -14014,7 +14010,7 @@
       <c r="CX6" s="28"/>
       <c r="CY6" s="28"/>
     </row>
-    <row r="7" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
@@ -14121,7 +14117,7 @@
       <c r="CX7" s="28"/>
       <c r="CY7" s="28"/>
     </row>
-    <row r="8" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -14228,7 +14224,7 @@
       <c r="CX8" s="28"/>
       <c r="CY8" s="28"/>
     </row>
-    <row r="9" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -14335,7 +14331,7 @@
       <c r="CX9" s="28"/>
       <c r="CY9" s="28"/>
     </row>
-    <row r="10" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -14442,7 +14438,7 @@
       <c r="CX10" s="28"/>
       <c r="CY10" s="28"/>
     </row>
-    <row r="11" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -14549,7 +14545,7 @@
       <c r="CX11" s="28"/>
       <c r="CY11" s="28"/>
     </row>
-    <row r="12" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
@@ -14656,7 +14652,7 @@
       <c r="CX12" s="28"/>
       <c r="CY12" s="28"/>
     </row>
-    <row r="13" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -14763,7 +14759,7 @@
       <c r="CX13" s="28"/>
       <c r="CY13" s="28"/>
     </row>
-    <row r="14" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
@@ -14870,7 +14866,7 @@
       <c r="CX14" s="28"/>
       <c r="CY14" s="28"/>
     </row>
-    <row r="15" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
@@ -14991,7 +14987,7 @@
       <c r="CX15" s="28"/>
       <c r="CY15" s="28"/>
     </row>
-    <row r="16" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
@@ -15106,7 +15102,7 @@
       <c r="CX16" s="28"/>
       <c r="CY16" s="28"/>
     </row>
-    <row r="17" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -15225,7 +15221,7 @@
       <c r="CX17" s="28"/>
       <c r="CY17" s="28"/>
     </row>
-    <row r="18" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -15347,7 +15343,7 @@
       <c r="CX18" s="28"/>
       <c r="CY18" s="28"/>
     </row>
-    <row r="19" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -15488,7 +15484,7 @@
       <c r="CX19" s="28"/>
       <c r="CY19" s="28"/>
     </row>
-    <row r="20" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="44" t="s">
         <v>9</v>
       </c>
@@ -15613,7 +15609,7 @@
       <c r="CX20" s="28"/>
       <c r="CY20" s="28"/>
     </row>
-    <row r="21" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="44" t="s">
         <v>0</v>
       </c>
@@ -15729,7 +15725,7 @@
       <c r="CX21" s="28"/>
       <c r="CY21" s="28"/>
     </row>
-    <row r="22" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -15858,7 +15854,7 @@
       <c r="CX22" s="28"/>
       <c r="CY22" s="28"/>
     </row>
-    <row r="23" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -15969,7 +15965,7 @@
       <c r="CX23" s="28"/>
       <c r="CY23" s="28"/>
     </row>
-    <row r="24" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -16081,7 +16077,7 @@
       <c r="CX24" s="28"/>
       <c r="CY24" s="28"/>
     </row>
-    <row r="25" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -16204,7 +16200,7 @@
       <c r="CX25" s="28"/>
       <c r="CY25" s="28"/>
     </row>
-    <row r="26" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -16333,7 +16329,7 @@
       <c r="CX26" s="28"/>
       <c r="CY26" s="28"/>
     </row>
-    <row r="27" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -16444,7 +16440,7 @@
       <c r="CX27" s="28"/>
       <c r="CY27" s="28"/>
     </row>
-    <row r="28" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -16553,7 +16549,7 @@
       <c r="CX28" s="28"/>
       <c r="CY28" s="28"/>
     </row>
-    <row r="29" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -16678,7 +16674,7 @@
       <c r="CX29" s="28"/>
       <c r="CY29" s="28"/>
     </row>
-    <row r="30" spans="1:103" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:103" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="54"/>
       <c r="B30" s="54"/>
       <c r="C30" s="54"/>
@@ -16785,7 +16781,7 @@
       <c r="CX30" s="28"/>
       <c r="CY30" s="28"/>
     </row>
-    <row r="31" spans="1:103" s="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:103" s="66" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC31" s="51">
         <v>29</v>
       </c>
@@ -16838,7 +16834,7 @@
       <c r="CX31" s="67"/>
       <c r="CY31" s="67"/>
     </row>
-    <row r="32" spans="1:103" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:103" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="53">
         <v>0</v>
       </c>
@@ -17051,7 +17047,7 @@
       <c r="CX32" s="28"/>
       <c r="CY32" s="28"/>
     </row>
-    <row r="33" spans="1:103" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:103" s="61" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="28"/>
       <c r="C33" s="28"/>
@@ -17156,7 +17152,7 @@
       <c r="CX33" s="28"/>
       <c r="CY33" s="28"/>
     </row>
-    <row r="34" spans="1:103" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:103" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J34" s="30"/>
       <c r="T34" s="31"/>
       <c r="AD34" s="32"/>
@@ -17164,7 +17160,7 @@
       <c r="AX34" s="34"/>
       <c r="BC34" s="35"/>
     </row>
-    <row r="35" spans="1:103" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:103" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
       <c r="B35" s="28"/>
       <c r="C35" s="28"/>
@@ -17269,7 +17265,7 @@
       <c r="CX35" s="28"/>
       <c r="CY35" s="28"/>
     </row>
-    <row r="36" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28"/>
       <c r="B36" s="28"/>
       <c r="C36" s="28"/>
@@ -17374,7 +17370,7 @@
       <c r="CX36" s="28"/>
       <c r="CY36" s="28"/>
     </row>
-    <row r="37" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28"/>
       <c r="B37" s="28"/>
       <c r="C37" s="28"/>
@@ -17479,7 +17475,7 @@
       <c r="CX37" s="28"/>
       <c r="CY37" s="28"/>
     </row>
-    <row r="38" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28"/>
       <c r="B38" s="28"/>
       <c r="C38" s="28"/>
@@ -17584,7 +17580,7 @@
       <c r="CX38" s="28"/>
       <c r="CY38" s="28"/>
     </row>
-    <row r="39" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28"/>
       <c r="B39" s="28"/>
       <c r="C39" s="28"/>
@@ -17689,7 +17685,7 @@
       <c r="CX39" s="28"/>
       <c r="CY39" s="28"/>
     </row>
-    <row r="40" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28"/>
       <c r="B40" s="28"/>
       <c r="C40" s="28"/>
@@ -17794,7 +17790,7 @@
       <c r="CX40" s="28"/>
       <c r="CY40" s="28"/>
     </row>
-    <row r="41" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28"/>
       <c r="B41" s="28"/>
       <c r="C41" s="28"/>
@@ -17899,7 +17895,7 @@
       <c r="CX41" s="28"/>
       <c r="CY41" s="28"/>
     </row>
-    <row r="42" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28"/>
       <c r="B42" s="28"/>
       <c r="C42" s="28"/>
@@ -18004,7 +18000,7 @@
       <c r="CX42" s="28"/>
       <c r="CY42" s="28"/>
     </row>
-    <row r="43" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28"/>
       <c r="B43" s="28"/>
       <c r="C43" s="28"/>
@@ -18109,7 +18105,7 @@
       <c r="CX43" s="28"/>
       <c r="CY43" s="28"/>
     </row>
-    <row r="44" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28"/>
       <c r="B44" s="28"/>
       <c r="C44" s="28"/>
@@ -18214,7 +18210,7 @@
       <c r="CX44" s="28"/>
       <c r="CY44" s="28"/>
     </row>
-    <row r="45" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="28"/>
       <c r="B45" s="28"/>
       <c r="C45" s="28"/>
@@ -18319,7 +18315,7 @@
       <c r="CX45" s="28"/>
       <c r="CY45" s="28"/>
     </row>
-    <row r="46" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28"/>
       <c r="B46" s="28"/>
       <c r="C46" s="28"/>
@@ -18424,7 +18420,7 @@
       <c r="CX46" s="28"/>
       <c r="CY46" s="28"/>
     </row>
-    <row r="47" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="BC47" s="41"/>
       <c r="BD47" s="42"/>
       <c r="BE47" s="42"/>
@@ -18488,9 +18484,9 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="62"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -18547,7 +18543,7 @@
       <c r="BB1" s="63"/>
       <c r="BC1" s="65"/>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -18606,7 +18602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -18665,7 +18661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -18724,7 +18720,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -18783,7 +18779,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -18842,7 +18838,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
@@ -18900,7 +18896,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -18981,7 +18977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -19062,7 +19058,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -19137,7 +19133,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -19212,7 +19208,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
@@ -19289,7 +19285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -19370,7 +19366,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" s="44"/>
       <c r="B14" s="44"/>
       <c r="C14" s="44"/>
@@ -19439,7 +19435,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" s="44"/>
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
@@ -19512,7 +19508,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
@@ -19575,7 +19571,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -19638,7 +19634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -19702,7 +19698,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A19" s="44" t="s">
         <v>0</v>
       </c>
@@ -19793,7 +19789,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -19854,7 +19850,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -19915,7 +19911,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -19976,7 +19972,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -20037,7 +20033,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -20098,7 +20094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A25" s="44" t="s">
         <v>9</v>
       </c>
@@ -20161,7 +20157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A26" s="44" t="s">
         <v>15</v>
       </c>
@@ -20238,7 +20234,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -20297,7 +20293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -20356,7 +20352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -20415,7 +20411,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A30" s="54"/>
       <c r="B30" s="54"/>
       <c r="C30" s="54"/>
@@ -20474,7 +20470,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="66"/>
       <c r="B31" s="66"/>
       <c r="C31" s="66"/>
@@ -20533,7 +20529,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A32" s="53">
         <v>0</v>
       </c>
@@ -20711,9 +20707,9 @@
       <selection activeCell="AQ22" sqref="AQ22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="4.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="62"/>
       <c r="B1" s="62"/>
       <c r="C1" s="62"/>
@@ -20770,7 +20766,7 @@
       <c r="BB1" s="63"/>
       <c r="BC1" s="65"/>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
       <c r="B2" s="44"/>
       <c r="C2" s="44"/>
@@ -20829,7 +20825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" s="44"/>
       <c r="B3" s="44"/>
       <c r="C3" s="44"/>
@@ -20888,7 +20884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="44"/>
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
@@ -20947,7 +20943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="44"/>
       <c r="B5" s="44"/>
       <c r="C5" s="44"/>
@@ -21006,7 +21002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="44"/>
       <c r="C6" s="44"/>
@@ -21065,7 +21061,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="44"/>
       <c r="C7" s="44"/>
@@ -21124,7 +21120,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
@@ -21163,7 +21159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -21202,7 +21198,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="44"/>
       <c r="C10" s="44"/>
@@ -21261,7 +21257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" s="44"/>
       <c r="B11" s="44"/>
       <c r="C11" s="44"/>
@@ -21317,7 +21313,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="44"/>
       <c r="B12" s="44"/>
       <c r="C12" s="44"/>
@@ -21368,7 +21364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" s="44"/>
       <c r="B13" s="44"/>
       <c r="C13" s="44"/>
@@ -21435,7 +21431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A14" s="44" t="s">
         <v>9</v>
       </c>
@@ -21504,7 +21500,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A15" s="44" t="s">
         <v>0</v>
       </c>
@@ -21591,7 +21587,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
       <c r="C16" s="44"/>
@@ -21674,7 +21670,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A17" s="44"/>
       <c r="B17" s="44"/>
       <c r="C17" s="44"/>
@@ -21745,7 +21741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A18" s="44"/>
       <c r="B18" s="44"/>
       <c r="C18" s="44"/>
@@ -21816,7 +21812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="44"/>
       <c r="C19" s="44"/>
@@ -21887,7 +21883,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="44"/>
       <c r="C20" s="44"/>
@@ -21967,7 +21963,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A21" s="44"/>
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
@@ -22040,7 +22036,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A22" s="44"/>
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
@@ -22106,7 +22102,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A23" s="44"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -22177,7 +22173,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A24" s="44"/>
       <c r="B24" s="44"/>
       <c r="C24" s="44"/>
@@ -22240,7 +22236,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="44"/>
@@ -22303,7 +22299,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A26" s="44"/>
       <c r="B26" s="44"/>
       <c r="C26" s="44"/>
@@ -22367,7 +22363,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A27" s="44"/>
       <c r="B27" s="44"/>
       <c r="C27" s="44"/>
@@ -22440,7 +22436,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A28" s="44"/>
       <c r="B28" s="44"/>
       <c r="C28" s="44"/>
@@ -22499,7 +22495,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -22558,7 +22554,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A30" s="54"/>
       <c r="B30" s="54"/>
       <c r="C30" s="54"/>
@@ -22617,7 +22613,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="66"/>
       <c r="B31" s="66"/>
       <c r="C31" s="66"/>
@@ -22676,7 +22672,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:55" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A32" s="53">
         <v>0</v>
       </c>

</xml_diff>